<commit_message>
update data extraction files and cleaning script
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/esther_beukhof_wur_nl/Documents/Projects/SEAwise/T4.1/Data extraction/Data extraction files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_C6C582AE6AA3174FCDCA3FC04E4E9F74C839F178" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7E885B50-BB50-4BC9-ADBD-B9F8CE9F80EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107CB41E-1E6B-424D-BF1E-2C1D9C1D9E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3495" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Drop-down overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$23</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -3320,9 +3321,6 @@
     <t>management measure of discard ban</t>
   </si>
   <si>
-    <t>consumption of discards</t>
-  </si>
-  <si>
     <t>SW4_0441</t>
   </si>
   <si>
@@ -3606,6 +3604,9 @@
   </si>
   <si>
     <t>catch per unit effort _ mature individuals per age _  growth parameters</t>
+  </si>
+  <si>
+    <t>Discarding during bottom trawl operations</t>
   </si>
 </sst>
 </file>
@@ -4064,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX17" sqref="AX17"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW25" sqref="AW25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4374,10 +4375,10 @@
         <v>69</v>
       </c>
       <c r="Y3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="Z3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AA3">
         <v>2</v>
@@ -4404,13 +4405,13 @@
         <v>148</v>
       </c>
       <c r="AL3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AM3" t="s">
         <v>231</v>
       </c>
       <c r="AO3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AQ3" t="s">
         <v>164</v>
@@ -4422,7 +4423,7 @@
         <v>255</v>
       </c>
       <c r="AU3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AV3" t="s">
         <v>113</v>
@@ -4533,7 +4534,7 @@
         <v>231</v>
       </c>
       <c r="AO4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ4" t="s">
         <v>164</v>
@@ -4548,7 +4549,7 @@
         <v>208</v>
       </c>
       <c r="AX4" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.3">
@@ -4652,7 +4653,7 @@
         <v>231</v>
       </c>
       <c r="AO5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AQ5" t="s">
         <v>164</v>
@@ -4756,7 +4757,7 @@
         <v>2</v>
       </c>
       <c r="AD6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AF6">
         <v>4.5</v>
@@ -4777,13 +4778,13 @@
         <v>148</v>
       </c>
       <c r="AL6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AM6" t="s">
         <v>231</v>
       </c>
       <c r="AO6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AQ6" t="s">
         <v>164</v>
@@ -4792,7 +4793,7 @@
         <v>281</v>
       </c>
       <c r="AU6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AV6" t="s">
         <v>206</v>
@@ -4801,7 +4802,7 @@
         <v>210</v>
       </c>
       <c r="AX6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.3">
@@ -4905,7 +4906,7 @@
         <v>231</v>
       </c>
       <c r="AO7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AQ7" t="s">
         <v>164</v>
@@ -5009,7 +5010,7 @@
         <v>2</v>
       </c>
       <c r="AD8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AF8">
         <v>4.5</v>
@@ -5030,13 +5031,13 @@
         <v>148</v>
       </c>
       <c r="AL8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AM8" t="s">
         <v>231</v>
       </c>
       <c r="AO8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AQ8" t="s">
         <v>164</v>
@@ -5045,7 +5046,7 @@
         <v>281</v>
       </c>
       <c r="AU8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AV8" t="s">
         <v>206</v>
@@ -5141,7 +5142,7 @@
         <v>2</v>
       </c>
       <c r="AD9" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF9" s="13">
         <v>4.4000000000000004</v>
@@ -5156,7 +5157,7 @@
         <v>144</v>
       </c>
       <c r="AL9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM9" t="s">
         <v>232</v>
@@ -5165,7 +5166,7 @@
         <v>160</v>
       </c>
       <c r="AO9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ9" t="s">
         <v>164</v>
@@ -5175,7 +5176,7 @@
       </c>
       <c r="AT9" s="11"/>
       <c r="AU9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV9" t="s">
         <v>199</v>
@@ -5184,7 +5185,7 @@
         <v>209</v>
       </c>
       <c r="AX9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.3">
@@ -5271,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="AD10" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF10" s="13">
         <v>4.4000000000000004</v>
@@ -5286,7 +5287,7 @@
         <v>144</v>
       </c>
       <c r="AL10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM10" t="s">
         <v>232</v>
@@ -5295,7 +5296,7 @@
         <v>160</v>
       </c>
       <c r="AO10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ10" t="s">
         <v>164</v>
@@ -5305,7 +5306,7 @@
       </c>
       <c r="AT10" s="11"/>
       <c r="AU10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV10" t="s">
         <v>199</v>
@@ -5314,7 +5315,7 @@
         <v>209</v>
       </c>
       <c r="AX10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.3">
@@ -5401,7 +5402,7 @@
         <v>2</v>
       </c>
       <c r="AD11" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF11" s="13">
         <v>4.4000000000000004</v>
@@ -5413,7 +5414,7 @@
         <v>118</v>
       </c>
       <c r="AL11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM11" t="s">
         <v>232</v>
@@ -5422,7 +5423,7 @@
         <v>160</v>
       </c>
       <c r="AO11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ11" t="s">
         <v>164</v>
@@ -5432,7 +5433,7 @@
       </c>
       <c r="AT11" s="11"/>
       <c r="AU11" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV11" t="s">
         <v>199</v>
@@ -5441,7 +5442,7 @@
         <v>209</v>
       </c>
       <c r="AX11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.3">
@@ -5528,7 +5529,7 @@
         <v>2</v>
       </c>
       <c r="AD12" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF12" s="13">
         <v>4.4000000000000004</v>
@@ -5540,7 +5541,7 @@
         <v>118</v>
       </c>
       <c r="AL12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM12" t="s">
         <v>232</v>
@@ -5549,7 +5550,7 @@
         <v>160</v>
       </c>
       <c r="AO12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ12" t="s">
         <v>164</v>
@@ -5559,7 +5560,7 @@
       </c>
       <c r="AT12" s="11"/>
       <c r="AU12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV12" t="s">
         <v>199</v>
@@ -5568,7 +5569,7 @@
         <v>209</v>
       </c>
       <c r="AX12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.3">
@@ -5655,7 +5656,7 @@
         <v>2</v>
       </c>
       <c r="AD13" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF13" s="13">
         <v>4.4000000000000004</v>
@@ -5670,7 +5671,7 @@
         <v>145</v>
       </c>
       <c r="AL13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM13" t="s">
         <v>232</v>
@@ -5679,7 +5680,7 @@
         <v>160</v>
       </c>
       <c r="AO13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ13" t="s">
         <v>164</v>
@@ -5689,7 +5690,7 @@
       </c>
       <c r="AT13" s="11"/>
       <c r="AU13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV13" t="s">
         <v>199</v>
@@ -5698,7 +5699,7 @@
         <v>209</v>
       </c>
       <c r="AX13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.3">
@@ -5785,7 +5786,7 @@
         <v>2</v>
       </c>
       <c r="AD14" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AF14" s="13">
         <v>4.4000000000000004</v>
@@ -5800,7 +5801,7 @@
         <v>145</v>
       </c>
       <c r="AL14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AM14" t="s">
         <v>232</v>
@@ -5809,7 +5810,7 @@
         <v>160</v>
       </c>
       <c r="AO14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ14" t="s">
         <v>164</v>
@@ -5819,7 +5820,7 @@
       </c>
       <c r="AT14" s="11"/>
       <c r="AU14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AV14" t="s">
         <v>199</v>
@@ -5828,7 +5829,7 @@
         <v>209</v>
       </c>
       <c r="AX14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.3">
@@ -5917,7 +5918,7 @@
         <v>306</v>
       </c>
       <c r="AF15">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG15" t="s">
         <v>107</v>
@@ -5932,7 +5933,7 @@
         <v>159</v>
       </c>
       <c r="AO15" t="s">
-        <v>310</v>
+        <v>405</v>
       </c>
       <c r="AP15" t="s">
         <v>309</v>
@@ -5950,16 +5951,16 @@
         <v>308</v>
       </c>
       <c r="AU15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AV15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AW15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AX15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.3">
@@ -6045,7 +6046,7 @@
         <v>2</v>
       </c>
       <c r="AD16" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AF16">
         <v>4.2</v>
@@ -6066,7 +6067,7 @@
         <v>162</v>
       </c>
       <c r="AO16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AQ16" t="s">
         <v>164</v>
@@ -6081,16 +6082,16 @@
         <v>308</v>
       </c>
       <c r="AU16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AV16" t="s">
         <v>238</v>
       </c>
       <c r="AW16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AX16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.3">
@@ -6176,10 +6177,10 @@
         <v>2</v>
       </c>
       <c r="AD17" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF17">
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG17" t="s">
         <v>107</v>
@@ -6194,7 +6195,7 @@
         <v>159</v>
       </c>
       <c r="AO17" t="s">
-        <v>310</v>
+        <v>405</v>
       </c>
       <c r="AP17" t="s">
         <v>309</v>
@@ -6212,57 +6213,57 @@
         <v>308</v>
       </c>
       <c r="AU17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AV17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AW17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AX17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B18" t="s">
         <v>243</v>
       </c>
       <c r="C18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D18" t="s">
         <v>312</v>
-      </c>
-      <c r="D18" t="s">
-        <v>313</v>
       </c>
       <c r="E18">
         <v>2018</v>
       </c>
       <c r="F18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G18" t="s">
         <v>314</v>
-      </c>
-      <c r="G18" t="s">
-        <v>315</v>
       </c>
       <c r="H18" t="s">
         <v>248</v>
       </c>
       <c r="I18" t="s">
+        <v>315</v>
+      </c>
+      <c r="J18" t="s">
         <v>316</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>317</v>
-      </c>
-      <c r="K18" t="s">
-        <v>318</v>
       </c>
       <c r="L18" t="s">
         <v>248</v>
       </c>
       <c r="M18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N18" t="s">
         <v>251</v>
@@ -6282,43 +6283,43 @@
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B19" t="s">
         <v>243</v>
       </c>
       <c r="C19" t="s">
+        <v>320</v>
+      </c>
+      <c r="D19" t="s">
         <v>321</v>
-      </c>
-      <c r="D19" t="s">
-        <v>322</v>
       </c>
       <c r="E19">
         <v>2013</v>
       </c>
       <c r="F19" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="H19" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="I19" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="J19" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="K19" s="12" t="s">
         <v>327</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>328</v>
       </c>
       <c r="L19" s="12" t="s">
         <v>248</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N19" t="s">
         <v>251</v>
@@ -6327,7 +6328,7 @@
         <v>252</v>
       </c>
       <c r="P19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q19" t="s">
         <v>21</v>
@@ -6351,7 +6352,7 @@
         <v>69</v>
       </c>
       <c r="Z19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AA19">
         <v>2</v>
@@ -6363,7 +6364,7 @@
         <v>2</v>
       </c>
       <c r="AD19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AF19">
         <v>4.2</v>
@@ -6378,7 +6379,7 @@
         <v>145</v>
       </c>
       <c r="AL19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AM19" t="s">
         <v>232</v>
@@ -6387,7 +6388,7 @@
         <v>160</v>
       </c>
       <c r="AO19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AQ19" t="s">
         <v>164</v>
@@ -6399,7 +6400,7 @@
         <v>175</v>
       </c>
       <c r="AU19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AV19" t="s">
         <v>199</v>
@@ -6408,48 +6409,48 @@
         <v>208</v>
       </c>
       <c r="AX19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B20" t="s">
         <v>243</v>
       </c>
       <c r="C20" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" t="s">
         <v>332</v>
-      </c>
-      <c r="D20" t="s">
-        <v>333</v>
       </c>
       <c r="E20">
         <v>2013</v>
       </c>
       <c r="F20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H20" t="s">
         <v>248</v>
       </c>
       <c r="I20" t="s">
+        <v>334</v>
+      </c>
+      <c r="J20" t="s">
         <v>335</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>336</v>
-      </c>
-      <c r="K20" t="s">
-        <v>337</v>
       </c>
       <c r="L20" t="s">
         <v>248</v>
       </c>
       <c r="M20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N20" t="s">
         <v>251</v>
@@ -6483,7 +6484,7 @@
         <v>69</v>
       </c>
       <c r="Z20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AA20">
         <v>2</v>
@@ -6495,7 +6496,7 @@
         <v>2</v>
       </c>
       <c r="AD20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AF20">
         <v>4.2</v>
@@ -6510,7 +6511,7 @@
         <v>144</v>
       </c>
       <c r="AL20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AM20" t="s">
         <v>232</v>
@@ -6519,7 +6520,7 @@
         <v>160</v>
       </c>
       <c r="AO20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ20" t="s">
         <v>164</v>
@@ -6531,7 +6532,7 @@
         <v>175</v>
       </c>
       <c r="AU20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AV20" t="s">
         <v>238</v>
@@ -6540,48 +6541,48 @@
         <v>208</v>
       </c>
       <c r="AX20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B21" t="s">
         <v>243</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D21" t="s">
         <v>340</v>
-      </c>
-      <c r="D21" t="s">
-        <v>341</v>
       </c>
       <c r="E21">
         <v>2012</v>
       </c>
       <c r="F21" t="s">
+        <v>341</v>
+      </c>
+      <c r="G21" t="s">
         <v>342</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>343</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>344</v>
-      </c>
-      <c r="I21" t="s">
-        <v>345</v>
       </c>
       <c r="J21" t="s">
         <v>273</v>
       </c>
       <c r="K21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L21" t="s">
         <v>248</v>
       </c>
       <c r="M21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N21" t="s">
         <v>251</v>
@@ -6607,43 +6608,43 @@
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B22" t="s">
         <v>243</v>
       </c>
       <c r="C22" t="s">
+        <v>348</v>
+      </c>
+      <c r="D22" t="s">
         <v>349</v>
-      </c>
-      <c r="D22" t="s">
-        <v>350</v>
       </c>
       <c r="E22">
         <v>2011</v>
       </c>
       <c r="F22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H22" t="s">
         <v>272</v>
       </c>
       <c r="I22" t="s">
+        <v>351</v>
+      </c>
+      <c r="J22" t="s">
         <v>352</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>353</v>
-      </c>
-      <c r="K22" t="s">
-        <v>354</v>
       </c>
       <c r="L22" t="s">
         <v>248</v>
       </c>
       <c r="M22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N22" t="s">
         <v>251</v>
@@ -6652,7 +6653,7 @@
         <v>252</v>
       </c>
       <c r="P22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q22" t="s">
         <v>21</v>
@@ -6677,7 +6678,7 @@
         <v>69</v>
       </c>
       <c r="Z22" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AA22">
         <v>2</v>
@@ -6689,7 +6690,7 @@
         <v>2</v>
       </c>
       <c r="AD22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AF22" s="12">
         <v>4.2</v>
@@ -6704,7 +6705,7 @@
         <v>144</v>
       </c>
       <c r="AL22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AM22" t="s">
         <v>232</v>
@@ -6713,13 +6714,13 @@
         <v>160</v>
       </c>
       <c r="AO22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ22" t="s">
         <v>150</v>
       </c>
       <c r="AU22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AV22" t="s">
         <v>238</v>
@@ -6728,30 +6729,30 @@
         <v>208</v>
       </c>
       <c r="AX22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B23" t="s">
         <v>243</v>
       </c>
       <c r="C23" t="s">
+        <v>356</v>
+      </c>
+      <c r="D23" t="s">
         <v>357</v>
-      </c>
-      <c r="D23" t="s">
-        <v>358</v>
       </c>
       <c r="E23">
         <v>1999</v>
       </c>
       <c r="F23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H23" t="s">
         <v>300</v>
@@ -6760,16 +6761,16 @@
         <v>300</v>
       </c>
       <c r="J23" t="s">
+        <v>359</v>
+      </c>
+      <c r="K23" t="s">
         <v>360</v>
-      </c>
-      <c r="K23" t="s">
-        <v>361</v>
       </c>
       <c r="L23" t="s">
         <v>248</v>
       </c>
       <c r="M23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N23" t="s">
         <v>251</v>
@@ -8900,12 +8901,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9023,15 +9021,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9053,16 +9061,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updata data extraction files and start figures manuscript
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107CB41E-1E6B-424D-BF1E-2C1D9C1D9E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF91E349-6553-4463-B48A-8DF3158C2C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="408">
   <si>
     <t>SearchID</t>
   </si>
@@ -3552,9 +3552,6 @@
     <t>Pagellus bogaraveo</t>
   </si>
   <si>
-    <t>Up to the mid-1970s, more than 15 000 t of blackspot sea bream were landed annually in Spanish and French ports. Thereafter, catches declined sharply from 1975 to 1985 and have stayed at low levels ever since.</t>
-  </si>
-  <si>
     <t>The average density of litter found on the seafloor of the Strait of Sicily decreased significantly, although slightly, from 2015 to 2019. Comparing the litter occurrence in the Strait of Sicily in the mid-The comparison of anthropic litter on trawlable bottoms of the Strait of Sicily in the mid-1990s with that found in the late 2010s showed an increase of the percentage of sites littered with single use and fishing-related waste.</t>
   </si>
   <si>
@@ -3603,10 +3600,19 @@
     <t>consumption of fisheries discards _ interspecific competition</t>
   </si>
   <si>
-    <t>catch per unit effort _ mature individuals per age _  growth parameters</t>
-  </si>
-  <si>
     <t>Discarding during bottom trawl operations</t>
+  </si>
+  <si>
+    <t>Spatial distribution</t>
+  </si>
+  <si>
+    <t>climate change</t>
+  </si>
+  <si>
+    <t>landings per unit effort _ mature individuals per age _  growth parameters _ spawning stock biomass</t>
+  </si>
+  <si>
+    <t>Up to the mid-1970s, more than 15 000 t of blackspot sea bream were landed annually in Spanish and French ports. Thereafter, catches declined sharply from 1975 to 1985 and have stayed at low levels ever since. Fishing mortalities of the main demersal stocks (hake, anglerfish, sole) were in the range 0.2–0.5 during the last 30 years. It is likely that the blackspot sea bream stock was exploited at a similar level, which is shown here to be unsustainable.</t>
   </si>
 </sst>
 </file>
@@ -4065,27 +4071,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AW25" sqref="AW25"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT32" sqref="AT32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="19" max="19" width="18.109375" customWidth="1"/>
-    <col min="24" max="25" width="32.5546875" customWidth="1"/>
-    <col min="34" max="35" width="17.5546875" customWidth="1"/>
-    <col min="36" max="36" width="18.5546875" customWidth="1"/>
-    <col min="37" max="37" width="19.109375" customWidth="1"/>
-    <col min="38" max="38" width="17.5546875" customWidth="1"/>
-    <col min="39" max="39" width="14.44140625" customWidth="1"/>
-    <col min="40" max="41" width="15.88671875" customWidth="1"/>
-    <col min="42" max="42" width="15.44140625" customWidth="1"/>
-    <col min="46" max="46" width="15.109375" customWidth="1"/>
-    <col min="47" max="47" width="18.5546875" customWidth="1"/>
+    <col min="19" max="19" width="18.08984375" customWidth="1"/>
+    <col min="24" max="25" width="32.54296875" customWidth="1"/>
+    <col min="34" max="35" width="17.54296875" customWidth="1"/>
+    <col min="36" max="36" width="18.54296875" customWidth="1"/>
+    <col min="37" max="37" width="19.08984375" customWidth="1"/>
+    <col min="38" max="38" width="17.54296875" customWidth="1"/>
+    <col min="39" max="39" width="14.453125" customWidth="1"/>
+    <col min="40" max="41" width="15.90625" customWidth="1"/>
+    <col min="42" max="42" width="15.453125" customWidth="1"/>
+    <col min="46" max="46" width="15.08984375" customWidth="1"/>
+    <col min="47" max="47" width="18.54296875" customWidth="1"/>
     <col min="48" max="48" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -4151,7 +4157,7 @@
       <c r="AW1" s="15"/>
       <c r="AX1" s="15"/>
     </row>
-    <row r="2" spans="1:50" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -4405,13 +4411,13 @@
         <v>148</v>
       </c>
       <c r="AL3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AM3" t="s">
         <v>231</v>
       </c>
       <c r="AO3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ3" t="s">
         <v>164</v>
@@ -4423,7 +4429,7 @@
         <v>255</v>
       </c>
       <c r="AU3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AV3" t="s">
         <v>113</v>
@@ -4435,7 +4441,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>257</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>231</v>
       </c>
       <c r="AO4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AQ4" t="s">
         <v>164</v>
@@ -4549,10 +4555,10 @@
         <v>208</v>
       </c>
       <c r="AX4" s="11" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>267</v>
       </c>
@@ -4653,7 +4659,7 @@
         <v>231</v>
       </c>
       <c r="AO5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AQ5" t="s">
         <v>164</v>
@@ -4674,7 +4680,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -4757,7 +4763,7 @@
         <v>2</v>
       </c>
       <c r="AD6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF6">
         <v>4.5</v>
@@ -4778,13 +4784,13 @@
         <v>148</v>
       </c>
       <c r="AL6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AM6" t="s">
         <v>231</v>
       </c>
       <c r="AO6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AQ6" t="s">
         <v>164</v>
@@ -4793,7 +4799,7 @@
         <v>281</v>
       </c>
       <c r="AU6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AV6" t="s">
         <v>206</v>
@@ -4802,10 +4808,10 @@
         <v>210</v>
       </c>
       <c r="AX6" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>267</v>
       </c>
@@ -4906,7 +4912,7 @@
         <v>231</v>
       </c>
       <c r="AO7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AQ7" t="s">
         <v>164</v>
@@ -4927,7 +4933,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>267</v>
       </c>
@@ -5010,7 +5016,7 @@
         <v>2</v>
       </c>
       <c r="AD8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF8">
         <v>4.5</v>
@@ -5031,13 +5037,13 @@
         <v>148</v>
       </c>
       <c r="AL8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AM8" t="s">
         <v>231</v>
       </c>
       <c r="AO8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AQ8" t="s">
         <v>164</v>
@@ -5046,7 +5052,7 @@
         <v>281</v>
       </c>
       <c r="AU8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AV8" t="s">
         <v>206</v>
@@ -5058,7 +5064,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -5157,7 +5163,7 @@
         <v>144</v>
       </c>
       <c r="AL9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM9" t="s">
         <v>232</v>
@@ -5166,7 +5172,7 @@
         <v>160</v>
       </c>
       <c r="AO9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ9" t="s">
         <v>164</v>
@@ -5188,7 +5194,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -5287,7 +5293,7 @@
         <v>144</v>
       </c>
       <c r="AL10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM10" t="s">
         <v>232</v>
@@ -5296,7 +5302,7 @@
         <v>160</v>
       </c>
       <c r="AO10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ10" t="s">
         <v>164</v>
@@ -5318,7 +5324,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>283</v>
       </c>
@@ -5414,7 +5420,7 @@
         <v>118</v>
       </c>
       <c r="AL11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM11" t="s">
         <v>232</v>
@@ -5423,7 +5429,7 @@
         <v>160</v>
       </c>
       <c r="AO11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ11" t="s">
         <v>164</v>
@@ -5445,7 +5451,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>283</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>118</v>
       </c>
       <c r="AL12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM12" t="s">
         <v>232</v>
@@ -5550,7 +5556,7 @@
         <v>160</v>
       </c>
       <c r="AO12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ12" t="s">
         <v>164</v>
@@ -5572,7 +5578,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>283</v>
       </c>
@@ -5671,7 +5677,7 @@
         <v>145</v>
       </c>
       <c r="AL13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM13" t="s">
         <v>232</v>
@@ -5680,7 +5686,7 @@
         <v>160</v>
       </c>
       <c r="AO13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ13" t="s">
         <v>164</v>
@@ -5702,7 +5708,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>283</v>
       </c>
@@ -5801,7 +5807,7 @@
         <v>145</v>
       </c>
       <c r="AL14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AM14" t="s">
         <v>232</v>
@@ -5810,7 +5816,7 @@
         <v>160</v>
       </c>
       <c r="AO14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AQ14" t="s">
         <v>164</v>
@@ -5832,7 +5838,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>295</v>
       </c>
@@ -5933,7 +5939,7 @@
         <v>159</v>
       </c>
       <c r="AO15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AP15" t="s">
         <v>309</v>
@@ -5963,7 +5969,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>295</v>
       </c>
@@ -6094,7 +6100,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>295</v>
       </c>
@@ -6195,7 +6201,7 @@
         <v>159</v>
       </c>
       <c r="AO17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="AP17" t="s">
         <v>309</v>
@@ -6213,7 +6219,7 @@
         <v>308</v>
       </c>
       <c r="AU17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AV17" t="s">
         <v>203</v>
@@ -6225,7 +6231,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>310</v>
       </c>
@@ -6281,7 +6287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>330</v>
       </c>
@@ -6520,7 +6526,10 @@
         <v>160</v>
       </c>
       <c r="AO20" t="s">
-        <v>399</v>
+        <v>398</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>405</v>
       </c>
       <c r="AQ20" t="s">
         <v>164</v>
@@ -6532,19 +6541,19 @@
         <v>175</v>
       </c>
       <c r="AU20" t="s">
-        <v>369</v>
+        <v>404</v>
       </c>
       <c r="AV20" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW20" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AX20" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -6606,7 +6615,7 @@
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>347</v>
       </c>
@@ -6714,25 +6723,25 @@
         <v>160</v>
       </c>
       <c r="AO22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ22" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="AU22" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="AV22" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW22" t="s">
         <v>208</v>
       </c>
       <c r="AX22" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="23" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>355</v>
       </c>
@@ -6921,17 +6930,17 @@
       <selection activeCell="AN24" sqref="AN24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="19" max="19" width="32.109375" customWidth="1"/>
-    <col min="23" max="23" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.08984375" customWidth="1"/>
+    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="32" max="32" width="14.5546875" customWidth="1"/>
-    <col min="33" max="33" width="26.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.54296875" customWidth="1"/>
+    <col min="33" max="33" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -6997,7 +7006,7 @@
       <c r="AW1" s="9"/>
       <c r="AX1" s="9"/>
     </row>
-    <row r="2" spans="1:50" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -7149,7 +7158,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
       <c r="Q3" t="s">
         <v>21</v>
       </c>
@@ -7206,7 +7215,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
       <c r="Q4" t="s">
         <v>22</v>
       </c>
@@ -7263,7 +7272,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R5" t="s">
         <v>83</v>
       </c>
@@ -7319,7 +7328,7 @@
       </c>
       <c r="AX5" s="8"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R6" t="s">
         <v>84</v>
       </c>
@@ -7364,7 +7373,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R7" t="s">
         <v>85</v>
       </c>
@@ -7406,7 +7415,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R8" t="s">
         <v>86</v>
       </c>
@@ -7444,7 +7453,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R9" t="s">
         <v>87</v>
       </c>
@@ -7479,7 +7488,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S10" t="s">
         <v>33</v>
       </c>
@@ -7511,7 +7520,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S11" t="s">
         <v>32</v>
       </c>
@@ -7546,7 +7555,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S12" t="s">
         <v>30</v>
       </c>
@@ -7578,7 +7587,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S13" t="s">
         <v>79</v>
       </c>
@@ -7613,7 +7622,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S14" t="s">
         <v>31</v>
       </c>
@@ -7642,7 +7651,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S15" t="s">
         <v>35</v>
       </c>
@@ -7671,7 +7680,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
       <c r="S16" t="s">
         <v>34</v>
       </c>
@@ -7691,7 +7700,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="17" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AM17" t="s">
         <v>162</v>
       </c>
@@ -7699,22 +7708,22 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="18" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AQ18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="19" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AQ19" s="7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="22" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH22" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="23" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH23" s="6" t="s">
         <v>115</v>
       </c>
@@ -7749,7 +7758,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="24" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH24" t="s">
         <v>129</v>
       </c>
@@ -7775,7 +7784,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="25" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH25" t="s">
         <v>137</v>
       </c>
@@ -7798,7 +7807,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="26" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AJ26" t="s">
         <v>144</v>
       </c>
@@ -7809,7 +7818,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="27" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AJ27" t="s">
         <v>147</v>
       </c>
@@ -7820,7 +7829,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="28" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AJ28" t="s">
         <v>149</v>
       </c>
@@ -7828,12 +7837,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="29" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AQ29" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="30" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH30" s="5" t="s">
         <v>151</v>
       </c>
@@ -7856,7 +7865,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="31" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH31" s="6" t="s">
         <v>129</v>
       </c>
@@ -7882,7 +7891,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="34:48" x14ac:dyDescent="0.3">
+    <row r="32" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH32" t="s">
         <v>153</v>
       </c>
@@ -7908,7 +7917,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="33" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AH33" t="s">
         <v>155</v>
       </c>
@@ -7928,7 +7937,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="34" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AI34" t="s">
         <v>157</v>
       </c>
@@ -7943,7 +7952,7 @@
       </c>
       <c r="AY34" s="7"/>
     </row>
-    <row r="35" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="35" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AI35" t="s">
         <v>113</v>
       </c>
@@ -7957,7 +7966,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="36" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AU36" t="s">
         <v>211</v>
       </c>
@@ -7965,10 +7974,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="37" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:51" x14ac:dyDescent="0.3">
+    <row r="38" spans="34:51" x14ac:dyDescent="0.35">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -7996,38 +8005,38 @@
       <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.54296875" customWidth="1"/>
+    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.90625" customWidth="1"/>
+    <col min="19" max="19" width="17.90625" customWidth="1"/>
+    <col min="20" max="20" width="19.453125" customWidth="1"/>
+    <col min="21" max="21" width="17.90625" customWidth="1"/>
+    <col min="22" max="22" width="18.54296875" customWidth="1"/>
+    <col min="26" max="26" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.44140625" customWidth="1"/>
-    <col min="30" max="30" width="15.109375" customWidth="1"/>
-    <col min="31" max="31" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.88671875" customWidth="1"/>
-    <col min="33" max="33" width="12.5546875" customWidth="1"/>
+    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.453125" customWidth="1"/>
+    <col min="30" max="30" width="15.08984375" customWidth="1"/>
+    <col min="31" max="31" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.90625" customWidth="1"/>
+    <col min="33" max="33" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -8074,7 +8083,7 @@
       <c r="AF1" s="15"/>
       <c r="AG1" s="15"/>
     </row>
-    <row r="2" spans="1:33" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -8175,7 +8184,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -8241,7 +8250,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -8292,7 +8301,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -8346,7 +8355,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -8388,7 +8397,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -8433,7 +8442,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -8471,7 +8480,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -8509,7 +8518,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -8544,7 +8553,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -8576,7 +8585,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -8608,7 +8617,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -8637,7 +8646,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -8660,7 +8669,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -8686,7 +8695,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -8703,7 +8712,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q17" t="s">
         <v>119</v>
       </c>
@@ -8714,7 +8723,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q18" t="s">
         <v>120</v>
       </c>
@@ -8728,7 +8737,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R19" t="s">
         <v>152</v>
       </c>
@@ -8742,7 +8751,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="17:28" x14ac:dyDescent="0.35">
       <c r="S20" t="s">
         <v>156</v>
       </c>
@@ -8753,7 +8762,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="17:28" x14ac:dyDescent="0.35">
       <c r="S21" t="s">
         <v>228</v>
       </c>
@@ -8767,7 +8776,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="17:28" x14ac:dyDescent="0.35">
       <c r="S22" t="s">
         <v>113</v>
       </c>
@@ -8778,7 +8787,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q23" t="s">
         <v>127</v>
       </c>
@@ -8789,7 +8798,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R24" t="s">
         <v>141</v>
       </c>
@@ -8797,7 +8806,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R25" t="s">
         <v>146</v>
       </c>
@@ -8805,7 +8814,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R26" t="s">
         <v>148</v>
       </c>
@@ -8813,7 +8822,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R27" t="s">
         <v>150</v>
       </c>
@@ -8827,7 +8836,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q28" t="s">
         <v>122</v>
       </c>
@@ -8838,7 +8847,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R29" t="s">
         <v>142</v>
       </c>
@@ -8849,7 +8858,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="30" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q30" t="s">
         <v>123</v>
       </c>
@@ -8860,7 +8869,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="17:28" x14ac:dyDescent="0.35">
       <c r="R31" t="s">
         <v>143</v>
       </c>
@@ -8868,7 +8877,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="17:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="17:28" x14ac:dyDescent="0.35">
       <c r="Q32" t="s">
         <v>128</v>
       </c>
@@ -8876,12 +8885,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="26:26" x14ac:dyDescent="0.35">
       <c r="Z33" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="26:26" x14ac:dyDescent="0.35">
       <c r="Z34" t="s">
         <v>150</v>
       </c>
@@ -8907,6 +8916,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -9020,31 +9038,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9058,12 +9075,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update data extraction files
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D79EC6-7FCA-410F-849A-C89130673421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13EF0E-9404-4563-A9E9-FA97E055ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Drop-down overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$28</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="409">
   <si>
     <t>SearchID</t>
   </si>
@@ -3522,9 +3522,6 @@
     <t>Squalus acanthias</t>
   </si>
   <si>
-    <t>stock assessment</t>
-  </si>
-  <si>
     <t>biomass index</t>
   </si>
   <si>
@@ -3616,6 +3613,9 @@
   </si>
   <si>
     <t>Questionnaire</t>
+  </si>
+  <si>
+    <t>commercial landings</t>
   </si>
 </sst>
 </file>
@@ -4072,10 +4072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX24"/>
+  <dimension ref="A1:AX28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AO30" sqref="AO30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4414,13 +4414,13 @@
         <v>148</v>
       </c>
       <c r="AL3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AM3" t="s">
         <v>231</v>
       </c>
       <c r="AO3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AQ3" t="s">
         <v>164</v>
@@ -4432,7 +4432,7 @@
         <v>255</v>
       </c>
       <c r="AU3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AV3" t="s">
         <v>113</v>
@@ -4537,7 +4537,7 @@
         <v>4.5</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AH4" t="s">
         <v>118</v>
@@ -4546,13 +4546,13 @@
         <v>148</v>
       </c>
       <c r="AL4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AM4" t="s">
         <v>231</v>
       </c>
       <c r="AO4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AQ4" t="s">
         <v>164</v>
@@ -4564,7 +4564,7 @@
         <v>255</v>
       </c>
       <c r="AU4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AV4" t="s">
         <v>113</v>
@@ -4675,7 +4675,7 @@
         <v>231</v>
       </c>
       <c r="AO5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AQ5" t="s">
         <v>164</v>
@@ -4690,7 +4690,7 @@
         <v>208</v>
       </c>
       <c r="AX5" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
@@ -4794,7 +4794,7 @@
         <v>231</v>
       </c>
       <c r="AO6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AQ6" t="s">
         <v>164</v>
@@ -4898,7 +4898,7 @@
         <v>2</v>
       </c>
       <c r="AD7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AF7">
         <v>4.5</v>
@@ -4919,13 +4919,13 @@
         <v>148</v>
       </c>
       <c r="AL7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AM7" t="s">
         <v>231</v>
       </c>
       <c r="AO7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AQ7" t="s">
         <v>164</v>
@@ -4934,7 +4934,7 @@
         <v>281</v>
       </c>
       <c r="AU7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AV7" t="s">
         <v>206</v>
@@ -4943,7 +4943,7 @@
         <v>210</v>
       </c>
       <c r="AX7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
@@ -5047,7 +5047,7 @@
         <v>231</v>
       </c>
       <c r="AO8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AQ8" t="s">
         <v>164</v>
@@ -5151,7 +5151,7 @@
         <v>2</v>
       </c>
       <c r="AD9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AF9">
         <v>4.5</v>
@@ -5172,13 +5172,13 @@
         <v>148</v>
       </c>
       <c r="AL9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AM9" t="s">
         <v>231</v>
       </c>
       <c r="AO9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AQ9" t="s">
         <v>164</v>
@@ -5187,7 +5187,7 @@
         <v>281</v>
       </c>
       <c r="AU9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AV9" t="s">
         <v>206</v>
@@ -5298,7 +5298,7 @@
         <v>144</v>
       </c>
       <c r="AL10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM10" t="s">
         <v>232</v>
@@ -5307,7 +5307,7 @@
         <v>160</v>
       </c>
       <c r="AO10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ10" t="s">
         <v>164</v>
@@ -5428,7 +5428,7 @@
         <v>144</v>
       </c>
       <c r="AL11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM11" t="s">
         <v>232</v>
@@ -5437,7 +5437,7 @@
         <v>160</v>
       </c>
       <c r="AO11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ11" t="s">
         <v>164</v>
@@ -5555,7 +5555,7 @@
         <v>118</v>
       </c>
       <c r="AL12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM12" t="s">
         <v>232</v>
@@ -5564,7 +5564,7 @@
         <v>160</v>
       </c>
       <c r="AO12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ12" t="s">
         <v>164</v>
@@ -5682,7 +5682,7 @@
         <v>118</v>
       </c>
       <c r="AL13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM13" t="s">
         <v>232</v>
@@ -5691,7 +5691,7 @@
         <v>160</v>
       </c>
       <c r="AO13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ13" t="s">
         <v>164</v>
@@ -5812,7 +5812,7 @@
         <v>145</v>
       </c>
       <c r="AL14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM14" t="s">
         <v>232</v>
@@ -5821,7 +5821,7 @@
         <v>160</v>
       </c>
       <c r="AO14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ14" t="s">
         <v>164</v>
@@ -5942,7 +5942,7 @@
         <v>145</v>
       </c>
       <c r="AL15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AM15" t="s">
         <v>232</v>
@@ -5951,7 +5951,7 @@
         <v>160</v>
       </c>
       <c r="AO15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AQ15" t="s">
         <v>164</v>
@@ -6074,7 +6074,7 @@
         <v>159</v>
       </c>
       <c r="AO16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AP16" t="s">
         <v>309</v>
@@ -6336,7 +6336,7 @@
         <v>159</v>
       </c>
       <c r="AO18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AP18" t="s">
         <v>309</v>
@@ -6354,7 +6354,7 @@
         <v>308</v>
       </c>
       <c r="AU18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AV18" t="s">
         <v>203</v>
@@ -6529,19 +6529,19 @@
         <v>160</v>
       </c>
       <c r="AO20" t="s">
-        <v>377</v>
+        <v>408</v>
       </c>
       <c r="AQ20" t="s">
         <v>164</v>
       </c>
       <c r="AR20" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="AS20" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="AU20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AV20" t="s">
         <v>199</v>
@@ -6550,48 +6550,48 @@
         <v>208</v>
       </c>
       <c r="AX20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B21" t="s">
         <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="E21">
         <v>2013</v>
       </c>
-      <c r="F21" t="s">
-        <v>313</v>
-      </c>
-      <c r="G21" t="s">
-        <v>333</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="F21" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L21" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="I21" t="s">
-        <v>334</v>
-      </c>
-      <c r="J21" t="s">
-        <v>335</v>
-      </c>
-      <c r="K21" t="s">
-        <v>336</v>
-      </c>
-      <c r="L21" t="s">
-        <v>248</v>
-      </c>
-      <c r="M21" t="s">
-        <v>337</v>
+      <c r="M21" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="N21" t="s">
         <v>251</v>
@@ -6600,32 +6600,31 @@
         <v>252</v>
       </c>
       <c r="P21" t="s">
-        <v>248</v>
+        <v>329</v>
       </c>
       <c r="Q21" t="s">
         <v>21</v>
       </c>
-      <c r="R21" s="12"/>
-      <c r="S21" t="s">
-        <v>24</v>
-      </c>
-      <c r="T21" t="s">
+      <c r="S21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="U21" t="s">
+      <c r="U21" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V21" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="W21" t="s">
+      <c r="W21" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="X21" t="s">
+      <c r="X21" s="12" t="s">
         <v>69</v>
       </c>
       <c r="Z21" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="AA21">
         <v>2</v>
@@ -6637,7 +6636,7 @@
         <v>2</v>
       </c>
       <c r="AD21" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="AF21">
         <v>4.2</v>
@@ -6646,13 +6645,13 @@
         <v>111</v>
       </c>
       <c r="AH21" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="AI21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL21" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="AM21" t="s">
         <v>232</v>
@@ -6661,72 +6660,69 @@
         <v>160</v>
       </c>
       <c r="AO21" t="s">
-        <v>398</v>
-      </c>
-      <c r="AP21" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="AQ21" t="s">
         <v>164</v>
       </c>
       <c r="AR21" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
       <c r="AS21" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="AU21" t="s">
-        <v>404</v>
+        <v>377</v>
       </c>
       <c r="AV21" t="s">
         <v>199</v>
       </c>
       <c r="AW21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AX21" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>338</v>
+        <v>319</v>
       </c>
       <c r="B22" t="s">
         <v>243</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>339</v>
+      <c r="C22" t="s">
+        <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="E22">
-        <v>2012</v>
-      </c>
-      <c r="F22" t="s">
-        <v>341</v>
-      </c>
-      <c r="G22" t="s">
-        <v>342</v>
-      </c>
-      <c r="H22" t="s">
-        <v>343</v>
-      </c>
-      <c r="I22" t="s">
-        <v>344</v>
-      </c>
-      <c r="J22" t="s">
-        <v>273</v>
-      </c>
-      <c r="K22" t="s">
-        <v>345</v>
-      </c>
-      <c r="L22" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L22" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="M22" t="s">
-        <v>346</v>
+      <c r="M22" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="N22" t="s">
         <v>251</v>
@@ -6735,60 +6731,126 @@
         <v>252</v>
       </c>
       <c r="P22" t="s">
-        <v>248</v>
+        <v>329</v>
       </c>
       <c r="Q22" t="s">
         <v>21</v>
       </c>
-      <c r="R22" t="s">
-        <v>84</v>
-      </c>
-      <c r="V22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AC22" s="12"/>
+      <c r="S22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V22" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA22">
+        <v>2</v>
+      </c>
+      <c r="AB22">
+        <v>2</v>
+      </c>
+      <c r="AC22">
+        <v>2</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>375</v>
+      </c>
+      <c r="AF22">
+        <v>4.2</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>376</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>408</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>239</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>377</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>347</v>
+        <v>319</v>
       </c>
       <c r="B23" t="s">
         <v>243</v>
       </c>
       <c r="C23" t="s">
-        <v>348</v>
+        <v>320</v>
       </c>
       <c r="D23" t="s">
-        <v>349</v>
+        <v>321</v>
       </c>
       <c r="E23">
-        <v>2011</v>
-      </c>
-      <c r="F23" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="G23" t="s">
-        <v>350</v>
-      </c>
-      <c r="H23" t="s">
-        <v>272</v>
-      </c>
-      <c r="I23" t="s">
-        <v>351</v>
-      </c>
-      <c r="J23" t="s">
-        <v>352</v>
-      </c>
-      <c r="K23" t="s">
-        <v>353</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="G23" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L23" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="M23" t="s">
-        <v>354</v>
+      <c r="M23" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="N23" t="s">
         <v>251</v>
@@ -6802,27 +6864,26 @@
       <c r="Q23" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="12"/>
-      <c r="S23" t="s">
+      <c r="S23" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="T23" t="s">
+      <c r="T23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="U23" t="s">
+      <c r="U23" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="W23" t="s">
+      <c r="W23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="X23" t="s">
+      <c r="X23" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="Z23" s="12" t="s">
-        <v>384</v>
+      <c r="Z23" t="s">
+        <v>374</v>
       </c>
       <c r="AA23">
         <v>2</v>
@@ -6834,37 +6895,40 @@
         <v>2</v>
       </c>
       <c r="AD23" t="s">
-        <v>385</v>
-      </c>
-      <c r="AF23" s="12">
+        <v>375</v>
+      </c>
+      <c r="AF23">
         <v>4.2</v>
       </c>
       <c r="AG23" t="s">
         <v>111</v>
       </c>
       <c r="AH23" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="AI23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL23" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="AM23" t="s">
         <v>232</v>
       </c>
       <c r="AN23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO23" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="AQ23" t="s">
         <v>164</v>
       </c>
+      <c r="AR23" t="s">
+        <v>169</v>
+      </c>
       <c r="AU23" t="s">
-        <v>406</v>
+        <v>377</v>
       </c>
       <c r="AV23" t="s">
         <v>199</v>
@@ -6873,48 +6937,48 @@
         <v>208</v>
       </c>
       <c r="AX23" t="s">
-        <v>407</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="B24" t="s">
         <v>243</v>
       </c>
       <c r="C24" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="D24" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
       <c r="E24">
-        <v>1999</v>
-      </c>
-      <c r="F24" t="s">
-        <v>313</v>
-      </c>
-      <c r="G24" t="s">
-        <v>358</v>
-      </c>
-      <c r="H24" t="s">
-        <v>300</v>
-      </c>
-      <c r="I24" t="s">
-        <v>300</v>
-      </c>
-      <c r="J24" t="s">
-        <v>359</v>
-      </c>
-      <c r="K24" t="s">
-        <v>360</v>
-      </c>
-      <c r="L24" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L24" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="M24" t="s">
-        <v>361</v>
+      <c r="M24" s="12" t="s">
+        <v>328</v>
       </c>
       <c r="N24" t="s">
         <v>251</v>
@@ -6923,15 +6987,469 @@
         <v>252</v>
       </c>
       <c r="P24" t="s">
-        <v>248</v>
+        <v>329</v>
       </c>
       <c r="Q24" t="s">
         <v>21</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="U24" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W24" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="X24" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA24">
+        <v>2</v>
+      </c>
+      <c r="AB24">
+        <v>2</v>
+      </c>
+      <c r="AC24">
+        <v>2</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>375</v>
+      </c>
+      <c r="AF24">
+        <v>4.2</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>376</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN24" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>408</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>188</v>
+      </c>
+      <c r="AU24" t="s">
+        <v>377</v>
+      </c>
+      <c r="AV24" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D25" t="s">
+        <v>332</v>
+      </c>
+      <c r="E25">
+        <v>2013</v>
+      </c>
+      <c r="F25" t="s">
+        <v>313</v>
+      </c>
+      <c r="G25" t="s">
+        <v>333</v>
+      </c>
+      <c r="H25" t="s">
+        <v>248</v>
+      </c>
+      <c r="I25" t="s">
+        <v>334</v>
+      </c>
+      <c r="J25" t="s">
+        <v>335</v>
+      </c>
+      <c r="K25" t="s">
+        <v>336</v>
+      </c>
+      <c r="L25" t="s">
+        <v>248</v>
+      </c>
+      <c r="M25" t="s">
+        <v>337</v>
+      </c>
+      <c r="N25" t="s">
+        <v>251</v>
+      </c>
+      <c r="O25" t="s">
+        <v>252</v>
+      </c>
+      <c r="P25" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R25" s="12"/>
+      <c r="S25" t="s">
+        <v>24</v>
+      </c>
+      <c r="T25" t="s">
+        <v>46</v>
+      </c>
+      <c r="U25" t="s">
+        <v>59</v>
+      </c>
+      <c r="V25" t="s">
+        <v>45</v>
+      </c>
+      <c r="W25" t="s">
+        <v>55</v>
+      </c>
+      <c r="X25" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>379</v>
+      </c>
+      <c r="AA25">
+        <v>2</v>
+      </c>
+      <c r="AB25">
+        <v>2</v>
+      </c>
+      <c r="AC25">
+        <v>2</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>380</v>
+      </c>
+      <c r="AF25">
+        <v>4.2</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI25" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>381</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN25" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>397</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>404</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU25" t="s">
+        <v>403</v>
+      </c>
+      <c r="AV25" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW25" t="s">
+        <v>210</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>338</v>
+      </c>
+      <c r="B26" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D26" t="s">
+        <v>340</v>
+      </c>
+      <c r="E26">
+        <v>2012</v>
+      </c>
+      <c r="F26" t="s">
+        <v>341</v>
+      </c>
+      <c r="G26" t="s">
+        <v>342</v>
+      </c>
+      <c r="H26" t="s">
+        <v>343</v>
+      </c>
+      <c r="I26" t="s">
+        <v>344</v>
+      </c>
+      <c r="J26" t="s">
+        <v>273</v>
+      </c>
+      <c r="K26" t="s">
+        <v>345</v>
+      </c>
+      <c r="L26" t="s">
+        <v>248</v>
+      </c>
+      <c r="M26" t="s">
+        <v>346</v>
+      </c>
+      <c r="N26" t="s">
+        <v>251</v>
+      </c>
+      <c r="O26" t="s">
+        <v>252</v>
+      </c>
+      <c r="P26" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26" t="s">
         <v>84</v>
       </c>
-      <c r="AF24" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>347</v>
+      </c>
+      <c r="B27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E27">
+        <v>2011</v>
+      </c>
+      <c r="F27" t="s">
+        <v>322</v>
+      </c>
+      <c r="G27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H27" t="s">
+        <v>272</v>
+      </c>
+      <c r="I27" t="s">
+        <v>351</v>
+      </c>
+      <c r="J27" t="s">
+        <v>352</v>
+      </c>
+      <c r="K27" t="s">
+        <v>353</v>
+      </c>
+      <c r="L27" t="s">
+        <v>248</v>
+      </c>
+      <c r="M27" t="s">
+        <v>354</v>
+      </c>
+      <c r="N27" t="s">
+        <v>251</v>
+      </c>
+      <c r="O27" t="s">
+        <v>252</v>
+      </c>
+      <c r="P27" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="12"/>
+      <c r="S27" t="s">
+        <v>25</v>
+      </c>
+      <c r="T27" t="s">
+        <v>46</v>
+      </c>
+      <c r="U27" t="s">
+        <v>59</v>
+      </c>
+      <c r="V27" t="s">
+        <v>45</v>
+      </c>
+      <c r="W27" t="s">
+        <v>55</v>
+      </c>
+      <c r="X27" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z27" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="AA27">
+        <v>2</v>
+      </c>
+      <c r="AB27">
+        <v>2</v>
+      </c>
+      <c r="AC27">
+        <v>2</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>384</v>
+      </c>
+      <c r="AF27" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI27" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>385</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN27" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO27" t="s">
+        <v>398</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>164</v>
+      </c>
+      <c r="AU27" t="s">
+        <v>405</v>
+      </c>
+      <c r="AV27" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX27" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" t="s">
+        <v>356</v>
+      </c>
+      <c r="D28" t="s">
+        <v>357</v>
+      </c>
+      <c r="E28">
+        <v>1999</v>
+      </c>
+      <c r="F28" t="s">
+        <v>313</v>
+      </c>
+      <c r="G28" t="s">
+        <v>358</v>
+      </c>
+      <c r="H28" t="s">
+        <v>300</v>
+      </c>
+      <c r="I28" t="s">
+        <v>300</v>
+      </c>
+      <c r="J28" t="s">
+        <v>359</v>
+      </c>
+      <c r="K28" t="s">
+        <v>360</v>
+      </c>
+      <c r="L28" t="s">
+        <v>248</v>
+      </c>
+      <c r="M28" t="s">
+        <v>361</v>
+      </c>
+      <c r="N28" t="s">
+        <v>251</v>
+      </c>
+      <c r="O28" t="s">
+        <v>252</v>
+      </c>
+      <c r="P28" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF28" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7649,7 +8167,7 @@
         <v>74</v>
       </c>
       <c r="AG10" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AH10" t="s">
         <v>119</v>
@@ -9054,14 +9572,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -9174,31 +9695,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47088D87-6CB8-4172-B6B3-6143CF4410FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -9214,9 +9725,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update data extraction files and creating new categories response variable
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Anastasopoulou.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13EF0E-9404-4563-A9E9-FA97E055ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA205C1-ACF5-4D51-9660-D99C0EFB7E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Drop-down overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$25</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="394">
   <si>
     <t>SearchID</t>
   </si>
@@ -3183,15 +3183,6 @@
     <t>Main findings: Higher density of litter distribution at deeper bottoms. Single-use and generic-use items accumulate along main shipping routes; fishing-related items are associated with specific fishing activities. © 2020 Elsevier LtdAbundance, composition, and distribution of macro-litter found on the seafloor of the Strait of Sicily between 10 and 800 m depth has been studied using data collected by bottom trawl surveys MEDITS from 2015 to 2019. Three waste categories based on the items use were considered: single-use, fishing-related and generic-use. Over 600 sampling sites, just 14% of these were litter-free. The five-years average density of seafloor litter was 79.6 items/km2 and ranged between 46.8 in 2019 and 118.1 items/km2 in 2015. The predominant waste type was plastic (58% of all items). Regardless of material type, single-use items were a dominant (60% of items) and widespread (79% of hauls) fraction of litter with a mean density of 48.4 items/km2. Fishing-related items accounted for 12% of total litter items. Percentage of dirty hauls and litter density increased with depth. Analysis of the relation density-depth indicates a progressive increase of litter density beyond depth values situated within the interval 234–477 m depending on the litter category. A significant decrease in litter density by categories was observed over the period. Patterns of spatial distribution at the higher depths (200–80 0m) resulted stable over the years. Density hotspots of fishing-related items were found where the fishing activity that uses fish aggregating devices (FADs) is practised and in the proximity of rocky banks. Single-use and generic-use objects densities were greater on the seafloor along main maritime routes than other areas. Comparisons between the percentage of hauls littered with anthropic waste from the mid-1990s against those in 2018–19 highlighted an increase of about 10.8% and 15.3% for single-use items and fishing-related items respectively, and a decrease of 18.6% for generic-use items. This study provides a snapshot of the current situation of littering in the central Mediterranean Sea and represents a solid baseline against which the effectiveness of current and future mitigation strategies of the litter impact on marine environment can be measured. © 2020 Elsevier Ltd</t>
   </si>
   <si>
-    <t>GLM with poisson distribution, distribution density indicators, increnebtak spatial autocorrelation</t>
-  </si>
-  <si>
-    <t>At least one item of litter was found in the 86% of sampling sites suggesting that pollution is rather ubiquitous in the area. waste originated from fishing activity (constituted by lost or dumped fishing gear) accounted for the 72% of total litter collected (60% and 12% respectively).Higher pollution  was observed at deeper bottoms compared to the depths belonging to the continental shelf (10-200 m).</t>
-  </si>
-  <si>
-    <t>density</t>
-  </si>
-  <si>
     <t>SW4_0933</t>
   </si>
   <si>
@@ -3228,18 +3219,6 @@
     <t>All Open Access, Gold, Green</t>
   </si>
   <si>
-    <t>PERMANOVA, SIMPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no relationship between the density and composition of debris and fishing intensity was detected. Moreover, the fishing debris (e.g. remains of fishing nets) was generally scarce and did not show significant differences regarding either the location or the sites with variable fishing activities. </t>
-  </si>
-  <si>
-    <t>surface dedge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the colonization of plastic debris by organisms might have further consequences for the functioning of the ecosystem </t>
-  </si>
-  <si>
     <t>SW4_0203</t>
   </si>
   <si>
@@ -3549,36 +3528,12 @@
     <t>Pagellus bogaraveo</t>
   </si>
   <si>
-    <t>The average density of litter found on the seafloor of the Strait of Sicily decreased significantly, although slightly, from 2015 to 2019. Comparing the litter occurrence in the Strait of Sicily in the mid-The comparison of anthropic litter on trawlable bottoms of the Strait of Sicily in the mid-1990s with that found in the late 2010s showed an increase of the percentage of sites littered with single use and fishing-related waste.</t>
-  </si>
-  <si>
     <t>Octopus vulgaris</t>
   </si>
   <si>
-    <t>More than 30% of plastics were between 10 and 20 cm width/length, and more than 40% of the plastics were colonized by a biofilm of microorganisms, suggesting indirect effects on benthic communities.</t>
-  </si>
-  <si>
-    <t>benthic communities</t>
-  </si>
-  <si>
-    <t>no interaction between the local epifaunal communities and marine debris could be detected.</t>
-  </si>
-  <si>
-    <t>organisms identification</t>
-  </si>
-  <si>
     <t>fish assemblages</t>
   </si>
   <si>
-    <t>litter colonization by organisms</t>
-  </si>
-  <si>
-    <t>litter categorization</t>
-  </si>
-  <si>
-    <t>composition and density of marine litter _ marine litter spatial distribution _ fraction of fisheries related litter _ time trend and relation to depth</t>
-  </si>
-  <si>
     <t>frequency of ML occurence inside octopus traps _ average number of ingested ML per individual _ identification of ingested plastics</t>
   </si>
   <si>
@@ -3591,9 +3546,6 @@
     <t>fishing hours</t>
   </si>
   <si>
-    <t>litter ingestion _ litter occurrence in the traps</t>
-  </si>
-  <si>
     <t>consumption of fisheries discards _ interspecific competition</t>
   </si>
   <si>
@@ -3616,6 +3568,9 @@
   </si>
   <si>
     <t>commercial landings</t>
+  </si>
+  <si>
+    <t>litter ingestion</t>
   </si>
 </sst>
 </file>
@@ -3741,7 +3696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3755,15 +3710,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4072,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX28"/>
+  <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO30" sqref="AO30"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AJ27" sqref="AJ27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4095,70 +4047,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="19" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="17" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="18" t="s">
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="20" t="s">
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="14" t="s">
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="15" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
     </row>
     <row r="2" spans="1:50" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4364,14 +4316,13 @@
       <c r="Q3" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="12"/>
       <c r="S3" t="s">
         <v>31</v>
       </c>
       <c r="T3" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" t="s">
         <v>55</v>
       </c>
       <c r="V3" t="s">
@@ -4384,10 +4335,10 @@
         <v>69</v>
       </c>
       <c r="Y3" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="Z3" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="AA3">
         <v>2</v>
@@ -4398,13 +4349,13 @@
       <c r="AC3">
         <v>2</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AD3" t="s">
         <v>254</v>
       </c>
       <c r="AF3">
         <v>4.5</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AG3" t="s">
         <v>109</v>
       </c>
       <c r="AH3" t="s">
@@ -4414,33 +4365,33 @@
         <v>148</v>
       </c>
       <c r="AL3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="AM3" t="s">
         <v>231</v>
       </c>
       <c r="AO3" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="AQ3" t="s">
         <v>164</v>
       </c>
       <c r="AR3" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="AT3" t="s">
         <v>255</v>
       </c>
       <c r="AU3" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="AV3" t="s">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="AW3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX3" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX3" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4496,14 +4447,13 @@
       <c r="Q4" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="12"/>
       <c r="S4" t="s">
         <v>31</v>
       </c>
       <c r="T4" t="s">
         <v>42</v>
       </c>
-      <c r="U4" s="12" t="s">
+      <c r="U4" t="s">
         <v>55</v>
       </c>
       <c r="V4" t="s">
@@ -4516,10 +4466,10 @@
         <v>69</v>
       </c>
       <c r="Y4" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="Z4" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="AA4">
         <v>2</v>
@@ -4530,14 +4480,14 @@
       <c r="AC4">
         <v>2</v>
       </c>
-      <c r="AD4" s="11" t="s">
+      <c r="AD4" t="s">
         <v>254</v>
       </c>
       <c r="AF4">
         <v>4.5</v>
       </c>
-      <c r="AG4" s="12" t="s">
-        <v>407</v>
+      <c r="AG4" t="s">
+        <v>391</v>
       </c>
       <c r="AH4" t="s">
         <v>118</v>
@@ -4546,33 +4496,33 @@
         <v>148</v>
       </c>
       <c r="AL4" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="AM4" t="s">
         <v>231</v>
       </c>
       <c r="AO4" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="AQ4" t="s">
         <v>164</v>
       </c>
       <c r="AR4" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="AT4" t="s">
         <v>255</v>
       </c>
       <c r="AU4" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="AV4" t="s">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="AW4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX4" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX4" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4625,268 +4575,144 @@
       <c r="Q5" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="12"/>
-      <c r="S5" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" t="s">
-        <v>57</v>
-      </c>
-      <c r="V5" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>264</v>
-      </c>
-      <c r="AA5">
-        <v>2</v>
-      </c>
-      <c r="AB5">
-        <v>2</v>
-      </c>
-      <c r="AC5">
-        <v>2</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>265</v>
+      <c r="R5" t="s">
+        <v>84</v>
       </c>
       <c r="AF5">
         <v>4.5</v>
       </c>
-      <c r="AG5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>231</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>395</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>113</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX5" s="11" t="s">
-        <v>386</v>
-      </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6">
         <v>2013</v>
       </c>
       <c r="F6" t="s">
+        <v>267</v>
+      </c>
+      <c r="G6" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" t="s">
+        <v>269</v>
+      </c>
+      <c r="I6" t="s">
         <v>270</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>271</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
         <v>272</v>
-      </c>
-      <c r="I6" t="s">
-        <v>273</v>
-      </c>
-      <c r="J6" t="s">
-        <v>274</v>
-      </c>
-      <c r="K6" t="s">
-        <v>275</v>
       </c>
       <c r="L6" t="s">
         <v>248</v>
       </c>
       <c r="M6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="N6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O6" t="s">
         <v>252</v>
       </c>
       <c r="P6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Q6" t="s">
         <v>21</v>
       </c>
-      <c r="S6" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" t="s">
-        <v>46</v>
-      </c>
-      <c r="U6" t="s">
-        <v>51</v>
-      </c>
-      <c r="V6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="X6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>279</v>
-      </c>
-      <c r="AA6">
-        <v>2</v>
-      </c>
-      <c r="AB6">
-        <v>2</v>
-      </c>
-      <c r="AC6">
-        <v>2</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>280</v>
+      <c r="R6" t="s">
+        <v>84</v>
       </c>
       <c r="AF6">
         <v>4.5</v>
       </c>
-      <c r="AG6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>231</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>394</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>164</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>281</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>266</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>282</v>
-      </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
         <v>243</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="E7">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="F7" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="G7" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="H7" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="I7" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="J7" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="K7" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="L7" t="s">
         <v>248</v>
       </c>
       <c r="M7" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N7" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="O7" t="s">
         <v>252</v>
       </c>
       <c r="P7" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="Q7" t="s">
         <v>21</v>
       </c>
       <c r="S7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="T7" t="s">
         <v>46</v>
       </c>
       <c r="U7" t="s">
-        <v>51</v>
-      </c>
-      <c r="V7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" t="s">
         <v>45</v>
       </c>
-      <c r="W7" s="12" t="s">
-        <v>47</v>
+      <c r="W7" t="s">
+        <v>55</v>
       </c>
       <c r="X7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z7" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="AA7">
         <v>2</v>
@@ -4898,126 +4724,123 @@
         <v>2</v>
       </c>
       <c r="AD7" t="s">
-        <v>388</v>
-      </c>
-      <c r="AF7">
-        <v>4.5</v>
+        <v>357</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AH7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AI7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AL7" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="AM7" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>160</v>
       </c>
       <c r="AO7" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="AQ7" t="s">
         <v>164</v>
       </c>
-      <c r="AT7" t="s">
-        <v>281</v>
+      <c r="AR7" t="s">
+        <v>239</v>
       </c>
       <c r="AU7" t="s">
-        <v>391</v>
+        <v>358</v>
       </c>
       <c r="AV7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AW7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AX7" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B8" t="s">
         <v>243</v>
       </c>
       <c r="C8" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="E8">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="G8" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="H8" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="I8" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="J8" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="K8" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="L8" t="s">
         <v>248</v>
       </c>
       <c r="M8" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N8" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="O8" t="s">
         <v>252</v>
       </c>
       <c r="P8" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="Q8" t="s">
         <v>21</v>
       </c>
       <c r="S8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T8" t="s">
         <v>46</v>
       </c>
       <c r="U8" t="s">
-        <v>51</v>
-      </c>
-      <c r="V8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
         <v>45</v>
       </c>
-      <c r="W8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="X8" s="12" t="s">
-        <v>216</v>
+      <c r="W8" t="s">
+        <v>55</v>
+      </c>
+      <c r="X8" t="s">
+        <v>215</v>
       </c>
       <c r="Z8" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="AA8">
         <v>2</v>
@@ -5029,117 +4852,123 @@
         <v>2</v>
       </c>
       <c r="AD8" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF8">
-        <v>4.5</v>
+        <v>357</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG8" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AH8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AI8" t="s">
-        <v>134</v>
+        <v>144</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>380</v>
       </c>
       <c r="AM8" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>160</v>
       </c>
       <c r="AO8" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="AQ8" t="s">
         <v>164</v>
       </c>
-      <c r="AT8" s="12" t="s">
-        <v>281</v>
+      <c r="AR8" t="s">
+        <v>240</v>
       </c>
       <c r="AU8" t="s">
-        <v>266</v>
+        <v>358</v>
       </c>
       <c r="AV8" t="s">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="AW8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AX8" t="s">
-        <v>282</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B9" t="s">
         <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="E9">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="F9" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="G9" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="I9" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="J9" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="K9" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="L9" t="s">
         <v>248</v>
       </c>
       <c r="M9" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N9" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="O9" t="s">
         <v>252</v>
       </c>
       <c r="P9" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="Q9" t="s">
         <v>21</v>
       </c>
       <c r="S9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T9" t="s">
         <v>46</v>
       </c>
       <c r="U9" t="s">
-        <v>51</v>
-      </c>
-      <c r="V9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V9" t="s">
         <v>45</v>
       </c>
-      <c r="W9" s="12" t="s">
-        <v>47</v>
+      <c r="W9" t="s">
+        <v>55</v>
       </c>
       <c r="X9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z9" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="AA9">
         <v>2</v>
@@ -5151,93 +4980,87 @@
         <v>2</v>
       </c>
       <c r="AD9" t="s">
-        <v>388</v>
-      </c>
-      <c r="AF9">
-        <v>4.5</v>
+        <v>357</v>
+      </c>
+      <c r="AF9" s="10">
+        <v>4.4000000000000004</v>
       </c>
       <c r="AG9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AH9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="AL9" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="AM9" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>160</v>
       </c>
       <c r="AO9" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="AQ9" t="s">
         <v>164</v>
       </c>
-      <c r="AT9" t="s">
-        <v>281</v>
+      <c r="AR9" t="s">
+        <v>239</v>
       </c>
       <c r="AU9" t="s">
-        <v>391</v>
+        <v>358</v>
       </c>
       <c r="AV9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AW9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AX9" t="s">
-        <v>282</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B10" t="s">
         <v>243</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E10">
         <v>2020</v>
       </c>
       <c r="F10" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G10" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H10" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="I10" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="J10" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="K10" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="L10" t="s">
         <v>248</v>
       </c>
       <c r="M10" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="N10" t="s">
         <v>251</v>
@@ -5246,12 +5069,11 @@
         <v>252</v>
       </c>
       <c r="P10" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="Q10" t="s">
         <v>21</v>
       </c>
-      <c r="R10" s="12"/>
       <c r="S10" t="s">
         <v>25</v>
       </c>
@@ -5271,7 +5093,7 @@
         <v>215</v>
       </c>
       <c r="Z10" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="AA10">
         <v>2</v>
@@ -5282,23 +5104,20 @@
       <c r="AC10">
         <v>2</v>
       </c>
-      <c r="AD10" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF10" s="13">
+      <c r="AD10" t="s">
+        <v>357</v>
+      </c>
+      <c r="AF10" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG10" t="s">
         <v>110</v>
       </c>
       <c r="AH10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="AL10" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="AM10" t="s">
         <v>232</v>
@@ -5307,17 +5126,16 @@
         <v>160</v>
       </c>
       <c r="AO10" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="AQ10" t="s">
         <v>164</v>
       </c>
       <c r="AR10" t="s">
-        <v>239</v>
-      </c>
-      <c r="AT10" s="11"/>
+        <v>240</v>
+      </c>
       <c r="AU10" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="AV10" t="s">
         <v>199</v>
@@ -5326,48 +5144,48 @@
         <v>209</v>
       </c>
       <c r="AX10" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B11" t="s">
         <v>243</v>
       </c>
       <c r="C11" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E11">
         <v>2020</v>
       </c>
       <c r="F11" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G11" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H11" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="I11" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="J11" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="K11" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="L11" t="s">
         <v>248</v>
       </c>
       <c r="M11" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="N11" t="s">
         <v>251</v>
@@ -5376,12 +5194,11 @@
         <v>252</v>
       </c>
       <c r="P11" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="Q11" t="s">
         <v>21</v>
       </c>
-      <c r="R11" s="12"/>
       <c r="S11" t="s">
         <v>25</v>
       </c>
@@ -5401,7 +5218,7 @@
         <v>215</v>
       </c>
       <c r="Z11" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="AA11">
         <v>2</v>
@@ -5412,23 +5229,23 @@
       <c r="AC11">
         <v>2</v>
       </c>
-      <c r="AD11" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF11" s="13">
+      <c r="AD11" t="s">
+        <v>357</v>
+      </c>
+      <c r="AF11" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG11" t="s">
         <v>110</v>
       </c>
       <c r="AH11" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="AI11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL11" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="AM11" t="s">
         <v>232</v>
@@ -5437,17 +5254,16 @@
         <v>160</v>
       </c>
       <c r="AO11" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="AQ11" t="s">
         <v>164</v>
       </c>
       <c r="AR11" t="s">
-        <v>240</v>
-      </c>
-      <c r="AT11" s="11"/>
+        <v>239</v>
+      </c>
       <c r="AU11" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="AV11" t="s">
         <v>199</v>
@@ -5456,48 +5272,48 @@
         <v>209</v>
       </c>
       <c r="AX11" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B12" t="s">
         <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E12">
         <v>2020</v>
       </c>
       <c r="F12" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G12" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H12" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="I12" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="J12" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="K12" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="L12" t="s">
         <v>248</v>
       </c>
       <c r="M12" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="N12" t="s">
         <v>251</v>
@@ -5506,12 +5322,11 @@
         <v>252</v>
       </c>
       <c r="P12" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="Q12" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="12"/>
       <c r="S12" t="s">
         <v>25</v>
       </c>
@@ -5531,7 +5346,7 @@
         <v>215</v>
       </c>
       <c r="Z12" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="AA12">
         <v>2</v>
@@ -5542,20 +5357,23 @@
       <c r="AC12">
         <v>2</v>
       </c>
-      <c r="AD12" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF12" s="13">
+      <c r="AD12" t="s">
+        <v>357</v>
+      </c>
+      <c r="AF12" s="10">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG12" t="s">
         <v>110</v>
       </c>
       <c r="AH12" t="s">
-        <v>118</v>
+        <v>220</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>145</v>
       </c>
       <c r="AL12" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="AM12" t="s">
         <v>232</v>
@@ -5564,17 +5382,16 @@
         <v>160</v>
       </c>
       <c r="AO12" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="AQ12" t="s">
         <v>164</v>
       </c>
       <c r="AR12" t="s">
-        <v>239</v>
-      </c>
-      <c r="AT12" s="11"/>
+        <v>240</v>
+      </c>
       <c r="AU12" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="AV12" t="s">
         <v>199</v>
@@ -5583,48 +5400,48 @@
         <v>209</v>
       </c>
       <c r="AX12" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B13" t="s">
         <v>243</v>
       </c>
       <c r="C13" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E13">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F13" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G13" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H13" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I13" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="J13" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="K13" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L13" t="s">
         <v>248</v>
       </c>
       <c r="M13" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="N13" t="s">
         <v>251</v>
@@ -5633,32 +5450,31 @@
         <v>252</v>
       </c>
       <c r="P13" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="Q13" t="s">
         <v>21</v>
       </c>
-      <c r="R13" s="12"/>
       <c r="S13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T13" t="s">
         <v>46</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="V13" t="s">
         <v>45</v>
       </c>
       <c r="W13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="X13" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="Z13" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="AA13">
         <v>2</v>
@@ -5669,45 +5485,50 @@
       <c r="AC13">
         <v>2</v>
       </c>
-      <c r="AD13" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF13" s="13">
+      <c r="AD13" t="s">
+        <v>299</v>
+      </c>
+      <c r="AF13">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AH13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AL13" t="s">
-        <v>392</v>
+        <v>298</v>
       </c>
       <c r="AM13" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AO13" t="s">
-        <v>399</v>
+        <v>386</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>302</v>
       </c>
       <c r="AQ13" t="s">
         <v>164</v>
       </c>
       <c r="AR13" t="s">
-        <v>240</v>
-      </c>
-      <c r="AT13" s="11"/>
+        <v>239</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>301</v>
+      </c>
       <c r="AU13" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AV13" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AW13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AX13" t="s">
         <v>366</v>
@@ -5715,43 +5536,43 @@
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B14" t="s">
         <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D14" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E14">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F14" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G14" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H14" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I14" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="J14" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="K14" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L14" t="s">
         <v>248</v>
       </c>
       <c r="M14" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="N14" t="s">
         <v>251</v>
@@ -5760,32 +5581,31 @@
         <v>252</v>
       </c>
       <c r="P14" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="Q14" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="12"/>
       <c r="S14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T14" t="s">
         <v>46</v>
       </c>
       <c r="U14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="V14" t="s">
         <v>45</v>
       </c>
       <c r="W14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="X14" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="Z14" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="AA14">
         <v>2</v>
@@ -5796,32 +5616,29 @@
       <c r="AC14">
         <v>2</v>
       </c>
-      <c r="AD14" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF14" s="13">
-        <v>4.4000000000000004</v>
+      <c r="AD14" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF14">
+        <v>4.2</v>
       </c>
       <c r="AG14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AH14" t="s">
-        <v>220</v>
-      </c>
-      <c r="AI14" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="AL14" t="s">
-        <v>392</v>
+        <v>298</v>
       </c>
       <c r="AM14" t="s">
         <v>232</v>
       </c>
       <c r="AN14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AO14" t="s">
-        <v>399</v>
+        <v>363</v>
       </c>
       <c r="AQ14" t="s">
         <v>164</v>
@@ -5829,59 +5646,64 @@
       <c r="AR14" t="s">
         <v>239</v>
       </c>
-      <c r="AT14" s="11"/>
+      <c r="AS14" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>301</v>
+      </c>
       <c r="AU14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AV14" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AX14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B15" t="s">
         <v>243</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E15">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="F15" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G15" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H15" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="I15" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="J15" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="K15" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L15" t="s">
         <v>248</v>
       </c>
       <c r="M15" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="N15" t="s">
         <v>251</v>
@@ -5890,32 +5712,31 @@
         <v>252</v>
       </c>
       <c r="P15" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="Q15" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="12"/>
       <c r="S15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T15" t="s">
         <v>46</v>
       </c>
       <c r="U15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="V15" t="s">
         <v>45</v>
       </c>
       <c r="W15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="X15" t="s">
-        <v>215</v>
+        <v>69</v>
       </c>
       <c r="Z15" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="AA15">
         <v>2</v>
@@ -5926,48 +5747,50 @@
       <c r="AC15">
         <v>2</v>
       </c>
-      <c r="AD15" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="AF15" s="13">
+      <c r="AD15" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF15">
         <v>4.4000000000000004</v>
       </c>
       <c r="AG15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AH15" t="s">
-        <v>220</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="AL15" t="s">
-        <v>392</v>
+        <v>300</v>
       </c>
       <c r="AM15" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AO15" t="s">
-        <v>399</v>
+        <v>386</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>302</v>
       </c>
       <c r="AQ15" t="s">
         <v>164</v>
       </c>
       <c r="AR15" t="s">
-        <v>240</v>
-      </c>
-      <c r="AT15" s="11"/>
+        <v>239</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>301</v>
+      </c>
       <c r="AU15" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="AV15" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AW15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AX15" t="s">
         <v>366</v>
@@ -5975,43 +5798,43 @@
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="B16" t="s">
         <v>243</v>
       </c>
       <c r="C16" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="D16" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="E16">
         <v>2018</v>
       </c>
       <c r="F16" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="G16" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="H16" t="s">
-        <v>300</v>
+        <v>248</v>
       </c>
       <c r="I16" t="s">
-        <v>248</v>
+        <v>308</v>
       </c>
       <c r="J16" t="s">
-        <v>248</v>
+        <v>309</v>
       </c>
       <c r="K16" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="L16" t="s">
         <v>248</v>
       </c>
       <c r="M16" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="N16" t="s">
         <v>251</v>
@@ -6020,129 +5843,54 @@
         <v>252</v>
       </c>
       <c r="P16" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="Q16" t="s">
         <v>21</v>
       </c>
-      <c r="S16" t="s">
-        <v>26</v>
-      </c>
-      <c r="T16" t="s">
-        <v>46</v>
-      </c>
-      <c r="U16" t="s">
-        <v>52</v>
-      </c>
-      <c r="V16" t="s">
-        <v>45</v>
-      </c>
-      <c r="W16" t="s">
-        <v>52</v>
-      </c>
-      <c r="X16" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>304</v>
-      </c>
-      <c r="AA16">
-        <v>2</v>
-      </c>
-      <c r="AB16">
-        <v>2</v>
-      </c>
-      <c r="AC16">
-        <v>2</v>
-      </c>
-      <c r="AD16" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="AF16">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>116</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>305</v>
-      </c>
-      <c r="AM16" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>402</v>
-      </c>
-      <c r="AP16" t="s">
-        <v>309</v>
-      </c>
-      <c r="AQ16" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR16" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS16" t="s">
-        <v>175</v>
-      </c>
-      <c r="AT16" t="s">
-        <v>308</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>367</v>
-      </c>
-      <c r="AV16" t="s">
-        <v>203</v>
-      </c>
-      <c r="AW16" t="s">
-        <v>207</v>
-      </c>
-      <c r="AX16" t="s">
-        <v>373</v>
+      <c r="R16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="B17" t="s">
         <v>243</v>
       </c>
       <c r="C17" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="D17" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="E17">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="F17" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="G17" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="H17" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="I17" t="s">
-        <v>248</v>
+        <v>318</v>
       </c>
       <c r="J17" t="s">
-        <v>248</v>
+        <v>319</v>
       </c>
       <c r="K17" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="L17" t="s">
         <v>248</v>
       </c>
       <c r="M17" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="N17" t="s">
         <v>251</v>
@@ -6151,31 +5899,31 @@
         <v>252</v>
       </c>
       <c r="P17" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="Q17" t="s">
         <v>21</v>
       </c>
       <c r="S17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T17" t="s">
         <v>46</v>
       </c>
       <c r="U17" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="V17" t="s">
         <v>45</v>
       </c>
       <c r="W17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="X17" t="s">
         <v>69</v>
       </c>
       <c r="Z17" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="AA17">
         <v>2</v>
@@ -6186,50 +5934,50 @@
       <c r="AC17">
         <v>2</v>
       </c>
-      <c r="AD17" s="11" t="s">
+      <c r="AD17" t="s">
         <v>368</v>
       </c>
       <c r="AF17">
         <v>4.2</v>
       </c>
       <c r="AG17" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AH17" t="s">
-        <v>116</v>
+        <v>220</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>145</v>
       </c>
       <c r="AL17" t="s">
-        <v>305</v>
-      </c>
-      <c r="AM17" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="AM17" t="s">
         <v>232</v>
       </c>
       <c r="AN17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO17" t="s">
-        <v>370</v>
+        <v>392</v>
       </c>
       <c r="AQ17" t="s">
         <v>164</v>
       </c>
       <c r="AR17" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="AS17" t="s">
-        <v>175</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>308</v>
+        <v>192</v>
       </c>
       <c r="AU17" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AV17" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AX17" t="s">
         <v>371</v>
@@ -6237,43 +5985,43 @@
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="B18" t="s">
         <v>243</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="D18" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="E18">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="F18" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="G18" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="H18" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>318</v>
       </c>
       <c r="J18" t="s">
-        <v>248</v>
+        <v>319</v>
       </c>
       <c r="K18" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="L18" t="s">
         <v>248</v>
       </c>
       <c r="M18" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="N18" t="s">
         <v>251</v>
@@ -6282,31 +6030,31 @@
         <v>252</v>
       </c>
       <c r="P18" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="Q18" t="s">
         <v>21</v>
       </c>
       <c r="S18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T18" t="s">
         <v>46</v>
       </c>
       <c r="U18" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="V18" t="s">
         <v>45</v>
       </c>
       <c r="W18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="X18" t="s">
         <v>69</v>
       </c>
       <c r="Z18" t="s">
-        <v>304</v>
+        <v>367</v>
       </c>
       <c r="AA18">
         <v>2</v>
@@ -6317,94 +6065,94 @@
       <c r="AC18">
         <v>2</v>
       </c>
-      <c r="AD18" s="11" t="s">
-        <v>372</v>
+      <c r="AD18" t="s">
+        <v>368</v>
       </c>
       <c r="AF18">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="AG18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AH18" t="s">
-        <v>116</v>
+        <v>220</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>145</v>
       </c>
       <c r="AL18" t="s">
-        <v>307</v>
-      </c>
-      <c r="AM18" s="12" t="s">
-        <v>159</v>
+        <v>369</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>160</v>
       </c>
       <c r="AO18" t="s">
-        <v>402</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>309</v>
+        <v>392</v>
       </c>
       <c r="AQ18" t="s">
         <v>164</v>
       </c>
       <c r="AR18" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
       <c r="AS18" t="s">
-        <v>175</v>
-      </c>
-      <c r="AT18" t="s">
-        <v>308</v>
+        <v>188</v>
       </c>
       <c r="AU18" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="AV18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="AW18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AX18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B19" t="s">
         <v>243</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D19" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E19">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="F19" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H19" t="s">
-        <v>248</v>
+        <v>317</v>
       </c>
       <c r="I19" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="J19" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="K19" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="L19" t="s">
         <v>248</v>
       </c>
       <c r="M19" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="N19" t="s">
         <v>251</v>
@@ -6413,54 +6161,126 @@
         <v>252</v>
       </c>
       <c r="P19" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="Q19" t="s">
         <v>21</v>
       </c>
-      <c r="R19" t="s">
-        <v>84</v>
+      <c r="S19" t="s">
+        <v>25</v>
+      </c>
+      <c r="T19" t="s">
+        <v>46</v>
+      </c>
+      <c r="U19" t="s">
+        <v>59</v>
+      </c>
+      <c r="V19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W19" t="s">
+        <v>55</v>
+      </c>
+      <c r="X19" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>367</v>
+      </c>
+      <c r="AA19">
+        <v>2</v>
+      </c>
+      <c r="AB19">
+        <v>2</v>
+      </c>
+      <c r="AC19">
+        <v>2</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>368</v>
+      </c>
+      <c r="AF19">
+        <v>4.2</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>369</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>392</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>239</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>370</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B20" t="s">
         <v>243</v>
       </c>
       <c r="C20" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D20" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E20">
         <v>2013</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="L20" s="12" t="s">
+      <c r="F20" t="s">
+        <v>315</v>
+      </c>
+      <c r="G20" t="s">
+        <v>316</v>
+      </c>
+      <c r="H20" t="s">
+        <v>317</v>
+      </c>
+      <c r="I20" t="s">
+        <v>318</v>
+      </c>
+      <c r="J20" t="s">
+        <v>319</v>
+      </c>
+      <c r="K20" t="s">
+        <v>320</v>
+      </c>
+      <c r="L20" t="s">
         <v>248</v>
       </c>
-      <c r="M20" s="12" t="s">
-        <v>328</v>
+      <c r="M20" t="s">
+        <v>321</v>
       </c>
       <c r="N20" t="s">
         <v>251</v>
@@ -6469,31 +6289,31 @@
         <v>252</v>
       </c>
       <c r="P20" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="Q20" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="12" t="s">
+      <c r="S20" t="s">
         <v>25</v>
       </c>
-      <c r="T20" s="12" t="s">
+      <c r="T20" t="s">
         <v>46</v>
       </c>
-      <c r="U20" s="12" t="s">
+      <c r="U20" t="s">
         <v>59</v>
       </c>
-      <c r="V20" s="12" t="s">
+      <c r="V20" t="s">
         <v>45</v>
       </c>
-      <c r="W20" s="12" t="s">
+      <c r="W20" t="s">
         <v>55</v>
       </c>
-      <c r="X20" s="12" t="s">
+      <c r="X20" t="s">
         <v>69</v>
       </c>
       <c r="Z20" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="AA20">
         <v>2</v>
@@ -6505,7 +6325,7 @@
         <v>2</v>
       </c>
       <c r="AD20" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="AF20">
         <v>4.2</v>
@@ -6520,28 +6340,25 @@
         <v>145</v>
       </c>
       <c r="AL20" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="AM20" t="s">
         <v>232</v>
       </c>
       <c r="AN20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO20" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="AQ20" t="s">
         <v>164</v>
       </c>
       <c r="AR20" t="s">
-        <v>197</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="AU20" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="AV20" t="s">
         <v>199</v>
@@ -6550,48 +6367,48 @@
         <v>208</v>
       </c>
       <c r="AX20" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B21" t="s">
         <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D21" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E21">
         <v>2013</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="F21" t="s">
+        <v>315</v>
+      </c>
+      <c r="G21" t="s">
+        <v>316</v>
+      </c>
+      <c r="H21" t="s">
+        <v>317</v>
+      </c>
+      <c r="I21" t="s">
+        <v>318</v>
+      </c>
+      <c r="J21" t="s">
+        <v>319</v>
+      </c>
+      <c r="K21" t="s">
+        <v>320</v>
+      </c>
+      <c r="L21" t="s">
         <v>248</v>
       </c>
-      <c r="M21" s="12" t="s">
-        <v>328</v>
+      <c r="M21" t="s">
+        <v>321</v>
       </c>
       <c r="N21" t="s">
         <v>251</v>
@@ -6600,31 +6417,31 @@
         <v>252</v>
       </c>
       <c r="P21" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="Q21" t="s">
         <v>21</v>
       </c>
-      <c r="S21" s="12" t="s">
+      <c r="S21" t="s">
         <v>25</v>
       </c>
-      <c r="T21" s="12" t="s">
+      <c r="T21" t="s">
         <v>46</v>
       </c>
-      <c r="U21" s="12" t="s">
+      <c r="U21" t="s">
         <v>59</v>
       </c>
-      <c r="V21" s="12" t="s">
+      <c r="V21" t="s">
         <v>45</v>
       </c>
-      <c r="W21" s="12" t="s">
+      <c r="W21" t="s">
         <v>55</v>
       </c>
-      <c r="X21" s="12" t="s">
+      <c r="X21" t="s">
         <v>69</v>
       </c>
       <c r="Z21" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="AA21">
         <v>2</v>
@@ -6636,7 +6453,7 @@
         <v>2</v>
       </c>
       <c r="AD21" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="AF21">
         <v>4.2</v>
@@ -6651,16 +6468,16 @@
         <v>145</v>
       </c>
       <c r="AL21" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="AM21" t="s">
         <v>232</v>
       </c>
       <c r="AN21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO21" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="AQ21" t="s">
         <v>164</v>
@@ -6672,7 +6489,7 @@
         <v>188</v>
       </c>
       <c r="AU21" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="AV21" t="s">
         <v>199</v>
@@ -6681,48 +6498,48 @@
         <v>208</v>
       </c>
       <c r="AX21" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B22" t="s">
         <v>243</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D22" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E22">
         <v>2013</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="J22" s="12" t="s">
+      <c r="F22" t="s">
+        <v>306</v>
+      </c>
+      <c r="G22" t="s">
         <v>326</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="H22" t="s">
+        <v>248</v>
+      </c>
+      <c r="I22" t="s">
         <v>327</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="J22" t="s">
+        <v>328</v>
+      </c>
+      <c r="K22" t="s">
+        <v>329</v>
+      </c>
+      <c r="L22" t="s">
         <v>248</v>
       </c>
-      <c r="M22" s="12" t="s">
-        <v>328</v>
+      <c r="M22" t="s">
+        <v>330</v>
       </c>
       <c r="N22" t="s">
         <v>251</v>
@@ -6731,31 +6548,31 @@
         <v>252</v>
       </c>
       <c r="P22" t="s">
-        <v>329</v>
+        <v>248</v>
       </c>
       <c r="Q22" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="T22" s="12" t="s">
+      <c r="S22" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" t="s">
         <v>46</v>
       </c>
-      <c r="U22" s="12" t="s">
+      <c r="U22" t="s">
         <v>59</v>
       </c>
-      <c r="V22" s="12" t="s">
+      <c r="V22" t="s">
         <v>45</v>
       </c>
-      <c r="W22" s="12" t="s">
+      <c r="W22" t="s">
         <v>55</v>
       </c>
-      <c r="X22" s="12" t="s">
+      <c r="X22" t="s">
         <v>69</v>
       </c>
       <c r="Z22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AA22">
         <v>2</v>
@@ -6767,7 +6584,7 @@
         <v>2</v>
       </c>
       <c r="AD22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF22">
         <v>4.2</v>
@@ -6776,22 +6593,25 @@
         <v>111</v>
       </c>
       <c r="AH22" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="AI22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AL22" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AM22" t="s">
         <v>232</v>
       </c>
       <c r="AN22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AO22" t="s">
-        <v>408</v>
+        <v>382</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>388</v>
       </c>
       <c r="AQ22" t="s">
         <v>164</v>
@@ -6799,58 +6619,61 @@
       <c r="AR22" t="s">
         <v>239</v>
       </c>
+      <c r="AS22" t="s">
+        <v>175</v>
+      </c>
       <c r="AU22" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="AV22" t="s">
         <v>199</v>
       </c>
       <c r="AW22" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AX22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="B23" t="s">
         <v>243</v>
       </c>
       <c r="C23" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D23" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="E23">
-        <v>2013</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="L23" s="12" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F23" t="s">
+        <v>334</v>
+      </c>
+      <c r="G23" t="s">
+        <v>335</v>
+      </c>
+      <c r="H23" t="s">
+        <v>336</v>
+      </c>
+      <c r="I23" t="s">
+        <v>337</v>
+      </c>
+      <c r="J23" t="s">
+        <v>270</v>
+      </c>
+      <c r="K23" t="s">
+        <v>338</v>
+      </c>
+      <c r="L23" t="s">
         <v>248</v>
       </c>
-      <c r="M23" s="12" t="s">
-        <v>328</v>
+      <c r="M23" t="s">
+        <v>339</v>
       </c>
       <c r="N23" t="s">
         <v>251</v>
@@ -6859,126 +6682,54 @@
         <v>252</v>
       </c>
       <c r="P23" t="s">
-        <v>329</v>
+        <v>248</v>
       </c>
       <c r="Q23" t="s">
         <v>21</v>
       </c>
-      <c r="S23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="U23" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="V23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="W23" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="X23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>374</v>
-      </c>
-      <c r="AA23">
-        <v>2</v>
-      </c>
-      <c r="AB23">
-        <v>2</v>
-      </c>
-      <c r="AC23">
-        <v>2</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>375</v>
-      </c>
-      <c r="AF23">
-        <v>4.2</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>220</v>
-      </c>
-      <c r="AI23" t="s">
-        <v>145</v>
-      </c>
-      <c r="AL23" t="s">
-        <v>376</v>
-      </c>
-      <c r="AM23" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN23" t="s">
-        <v>161</v>
-      </c>
-      <c r="AO23" t="s">
-        <v>408</v>
-      </c>
-      <c r="AQ23" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR23" t="s">
-        <v>169</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>377</v>
-      </c>
-      <c r="AV23" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX23" t="s">
-        <v>378</v>
+      <c r="R23" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="B24" t="s">
         <v>243</v>
       </c>
       <c r="C24" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="D24" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="E24">
-        <v>2013</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="L24" s="12" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F24" t="s">
+        <v>315</v>
+      </c>
+      <c r="G24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" t="s">
+        <v>344</v>
+      </c>
+      <c r="J24" t="s">
+        <v>345</v>
+      </c>
+      <c r="K24" t="s">
+        <v>346</v>
+      </c>
+      <c r="L24" t="s">
         <v>248</v>
       </c>
-      <c r="M24" s="12" t="s">
-        <v>328</v>
+      <c r="M24" t="s">
+        <v>347</v>
       </c>
       <c r="N24" t="s">
         <v>251</v>
@@ -6987,31 +6738,31 @@
         <v>252</v>
       </c>
       <c r="P24" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="Q24" t="s">
         <v>21</v>
       </c>
-      <c r="S24" s="12" t="s">
+      <c r="S24" t="s">
         <v>25</v>
       </c>
-      <c r="T24" s="12" t="s">
+      <c r="T24" t="s">
         <v>46</v>
       </c>
-      <c r="U24" s="12" t="s">
+      <c r="U24" t="s">
         <v>59</v>
       </c>
-      <c r="V24" s="12" t="s">
+      <c r="V24" t="s">
         <v>45</v>
       </c>
-      <c r="W24" s="12" t="s">
+      <c r="W24" t="s">
         <v>55</v>
       </c>
-      <c r="X24" s="12" t="s">
+      <c r="X24" t="s">
         <v>69</v>
       </c>
       <c r="Z24" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AA24">
         <v>2</v>
@@ -7023,7 +6774,7 @@
         <v>2</v>
       </c>
       <c r="AD24" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AF24">
         <v>4.2</v>
@@ -7032,34 +6783,28 @@
         <v>111</v>
       </c>
       <c r="AH24" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="AI24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AL24" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AM24" t="s">
         <v>232</v>
       </c>
       <c r="AN24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AO24" t="s">
-        <v>408</v>
+        <v>383</v>
       </c>
       <c r="AQ24" t="s">
         <v>164</v>
       </c>
-      <c r="AR24" t="s">
-        <v>170</v>
-      </c>
-      <c r="AS24" t="s">
-        <v>188</v>
-      </c>
       <c r="AU24" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="AV24" t="s">
         <v>199</v>
@@ -7068,48 +6813,48 @@
         <v>208</v>
       </c>
       <c r="AX24" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="B25" t="s">
         <v>243</v>
       </c>
       <c r="C25" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="D25" t="s">
-        <v>332</v>
+        <v>350</v>
       </c>
       <c r="E25">
-        <v>2013</v>
+        <v>1999</v>
       </c>
       <c r="F25" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="G25" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="H25" t="s">
-        <v>248</v>
+        <v>293</v>
       </c>
       <c r="I25" t="s">
-        <v>334</v>
+        <v>293</v>
       </c>
       <c r="J25" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="K25" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="L25" t="s">
         <v>248</v>
       </c>
       <c r="M25" t="s">
-        <v>337</v>
+        <v>354</v>
       </c>
       <c r="N25" t="s">
         <v>251</v>
@@ -7123,333 +6868,9 @@
       <c r="Q25" t="s">
         <v>21</v>
       </c>
-      <c r="R25" s="12"/>
-      <c r="S25" t="s">
-        <v>24</v>
-      </c>
-      <c r="T25" t="s">
-        <v>46</v>
-      </c>
-      <c r="U25" t="s">
-        <v>59</v>
-      </c>
-      <c r="V25" t="s">
-        <v>45</v>
-      </c>
-      <c r="W25" t="s">
-        <v>55</v>
-      </c>
-      <c r="X25" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>379</v>
-      </c>
-      <c r="AA25">
-        <v>2</v>
-      </c>
-      <c r="AB25">
-        <v>2</v>
-      </c>
-      <c r="AC25">
-        <v>2</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>380</v>
-      </c>
-      <c r="AF25">
-        <v>4.2</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI25" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL25" t="s">
-        <v>381</v>
-      </c>
-      <c r="AM25" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN25" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO25" t="s">
-        <v>397</v>
-      </c>
-      <c r="AP25" t="s">
-        <v>404</v>
-      </c>
-      <c r="AQ25" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR25" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS25" t="s">
-        <v>175</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>403</v>
-      </c>
-      <c r="AV25" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>210</v>
-      </c>
-      <c r="AX25" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>338</v>
-      </c>
-      <c r="B26" t="s">
-        <v>243</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="D26" t="s">
-        <v>340</v>
-      </c>
-      <c r="E26">
-        <v>2012</v>
-      </c>
-      <c r="F26" t="s">
-        <v>341</v>
-      </c>
-      <c r="G26" t="s">
-        <v>342</v>
-      </c>
-      <c r="H26" t="s">
-        <v>343</v>
-      </c>
-      <c r="I26" t="s">
-        <v>344</v>
-      </c>
-      <c r="J26" t="s">
-        <v>273</v>
-      </c>
-      <c r="K26" t="s">
-        <v>345</v>
-      </c>
-      <c r="L26" t="s">
-        <v>248</v>
-      </c>
-      <c r="M26" t="s">
-        <v>346</v>
-      </c>
-      <c r="N26" t="s">
-        <v>251</v>
-      </c>
-      <c r="O26" t="s">
-        <v>252</v>
-      </c>
-      <c r="P26" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>21</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="R25" t="s">
         <v>84</v>
       </c>
-      <c r="V26" s="12"/>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>347</v>
-      </c>
-      <c r="B27" t="s">
-        <v>243</v>
-      </c>
-      <c r="C27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D27" t="s">
-        <v>349</v>
-      </c>
-      <c r="E27">
-        <v>2011</v>
-      </c>
-      <c r="F27" t="s">
-        <v>322</v>
-      </c>
-      <c r="G27" t="s">
-        <v>350</v>
-      </c>
-      <c r="H27" t="s">
-        <v>272</v>
-      </c>
-      <c r="I27" t="s">
-        <v>351</v>
-      </c>
-      <c r="J27" t="s">
-        <v>352</v>
-      </c>
-      <c r="K27" t="s">
-        <v>353</v>
-      </c>
-      <c r="L27" t="s">
-        <v>248</v>
-      </c>
-      <c r="M27" t="s">
-        <v>354</v>
-      </c>
-      <c r="N27" t="s">
-        <v>251</v>
-      </c>
-      <c r="O27" t="s">
-        <v>252</v>
-      </c>
-      <c r="P27" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>21</v>
-      </c>
-      <c r="R27" s="12"/>
-      <c r="S27" t="s">
-        <v>25</v>
-      </c>
-      <c r="T27" t="s">
-        <v>46</v>
-      </c>
-      <c r="U27" t="s">
-        <v>59</v>
-      </c>
-      <c r="V27" t="s">
-        <v>45</v>
-      </c>
-      <c r="W27" t="s">
-        <v>55</v>
-      </c>
-      <c r="X27" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z27" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="AA27">
-        <v>2</v>
-      </c>
-      <c r="AB27">
-        <v>2</v>
-      </c>
-      <c r="AC27">
-        <v>2</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>384</v>
-      </c>
-      <c r="AF27" s="12">
-        <v>4.2</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>144</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>385</v>
-      </c>
-      <c r="AM27" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN27" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO27" t="s">
-        <v>398</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>164</v>
-      </c>
-      <c r="AU27" t="s">
-        <v>405</v>
-      </c>
-      <c r="AV27" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW27" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX27" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>355</v>
-      </c>
-      <c r="B28" t="s">
-        <v>243</v>
-      </c>
-      <c r="C28" t="s">
-        <v>356</v>
-      </c>
-      <c r="D28" t="s">
-        <v>357</v>
-      </c>
-      <c r="E28">
-        <v>1999</v>
-      </c>
-      <c r="F28" t="s">
-        <v>313</v>
-      </c>
-      <c r="G28" t="s">
-        <v>358</v>
-      </c>
-      <c r="H28" t="s">
-        <v>300</v>
-      </c>
-      <c r="I28" t="s">
-        <v>300</v>
-      </c>
-      <c r="J28" t="s">
-        <v>359</v>
-      </c>
-      <c r="K28" t="s">
-        <v>360</v>
-      </c>
-      <c r="L28" t="s">
-        <v>248</v>
-      </c>
-      <c r="M28" t="s">
-        <v>361</v>
-      </c>
-      <c r="N28" t="s">
-        <v>251</v>
-      </c>
-      <c r="O28" t="s">
-        <v>252</v>
-      </c>
-      <c r="P28" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>21</v>
-      </c>
-      <c r="R28" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF28" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7462,14 +6883,14 @@
     <mergeCell ref="AM1:AP1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="Q3:Q15 P16:P1048576" xr:uid="{F0DBF842-21D3-4EFA-92C7-9DB86B41273E}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="P13:P1048576 Q3:Q12" xr:uid="{F0DBF842-21D3-4EFA-92C7-9DB86B41273E}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3:AH1048576" xr:uid="{C4E6CF40-7606-499A-BCDE-5A81824A29A0}">
       <formula1>Ecosystem_component</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ3:AQ1048576" xr:uid="{AD1C325B-72C2-4B06-B4DE-534E7AB01CFB}">
       <formula1>Fishery_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN3:AN1048576 AI3:AJ1048576 AR3:AS1048576" xr:uid="{6349C90E-FB16-4F74-BDBE-2F3BA6CF0347}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR3:AS1048576 AI3:AJ1048576 AN3:AN1048576" xr:uid="{6349C90E-FB16-4F74-BDBE-2F3BA6CF0347}">
       <formula1>INDIRECT(AH3)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7479,6 +6900,18 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F8B7609-00EE-4B2C-B5EE-A85B819131B5}">
+          <x14:formula1>
+            <xm:f>Validation!$AG$3:$AG$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG3 AG5:AG1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D727A82-7958-4663-BF04-074CE15F93CE}">
+          <x14:formula1>
+            <xm:f>Validation!$AG$3:$AG$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG4</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBE6481C-F28A-47CE-9052-EC0DA42D6953}">
           <x14:formula1>
             <xm:f>Validation!$AM$5:$AM$11</xm:f>
@@ -7539,12 +6972,6 @@
           </x14:formula1>
           <xm:sqref>AC3:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F8B7609-00EE-4B2C-B5EE-A85B819131B5}">
-          <x14:formula1>
-            <xm:f>Validation!$AG$3:$AG$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>AG3 AG5:AG1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99A651E9-256A-4481-BED2-5B5E865E15C4}">
           <x14:formula1>
             <xm:f>Validation!$AK$3:$AK$7</xm:f>
@@ -7569,12 +6996,6 @@
           </x14:formula1>
           <xm:sqref>AV3:AV1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D727A82-7958-4663-BF04-074CE15F93CE}">
-          <x14:formula1>
-            <xm:f>Validation!$AG$3:$AG$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>AG4</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -7583,7 +7004,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AY38"/>
+  <dimension ref="A1:AX38"/>
   <sheetViews>
     <sheetView topLeftCell="Z1" workbookViewId="0">
       <selection activeCell="AG11" sqref="AG11"/>
@@ -7600,70 +7021,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="19" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="17" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="18" t="s">
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="10" t="s">
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="14" t="s">
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="9" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
     </row>
     <row r="2" spans="1:50" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -7985,7 +7406,7 @@
       <c r="AW5" t="s">
         <v>210</v>
       </c>
-      <c r="AX5" s="8"/>
+      <c r="AX5" s="7"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.35">
       <c r="R6" t="s">
@@ -8167,7 +7588,7 @@
         <v>74</v>
       </c>
       <c r="AG10" s="4" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="AH10" t="s">
         <v>119</v>
@@ -8376,7 +7797,7 @@
       </c>
     </row>
     <row r="19" spans="34:48" x14ac:dyDescent="0.35">
-      <c r="AQ19" s="7" t="s">
+      <c r="AQ19" t="s">
         <v>113</v>
       </c>
     </row>
@@ -8579,7 +8000,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="33" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AH33" t="s">
         <v>155</v>
       </c>
@@ -8599,7 +8020,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="34" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AI34" t="s">
         <v>157</v>
       </c>
@@ -8612,9 +8033,8 @@
       <c r="AV34" t="s">
         <v>194</v>
       </c>
-      <c r="AY34" s="7"/>
-    </row>
-    <row r="35" spans="34:51" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AI35" t="s">
         <v>113</v>
       </c>
@@ -8628,7 +8048,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="36" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AU36" t="s">
         <v>211</v>
       </c>
@@ -8636,10 +8056,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="37" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:51" x14ac:dyDescent="0.35">
+    <row r="38" spans="34:48" x14ac:dyDescent="0.35">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -8699,51 +8119,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="17" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="18" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="10" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="14" t="s">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="15" t="s">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
     </row>
     <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -9266,7 +8686,7 @@
       <c r="G12" t="s">
         <v>76</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" t="s">
         <v>221</v>
       </c>
       <c r="R12" t="s">
@@ -9581,6 +9001,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -9694,12 +9120,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
@@ -9709,6 +9129,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47088D87-6CB8-4172-B6B3-6143CF4410FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9722,19 +9157,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>